<commit_message>
Updated USA model - 2025-07-29 08:47
</commit_message>
<xml_diff>
--- a/VerveStacks_USA/SuppXLS/Scen_Par-NGFS.xlsx
+++ b/VerveStacks_USA/SuppXLS/Scen_Par-NGFS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_USA\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB5BFEF-7105-4B1A-B30C-69E3A97C6865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A8EFD71-D493-4FAA-966C-6ADF4C8E3AFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="84">
   <si>
     <t>~Inputcell: 3</t>
   </si>
@@ -284,6 +284,9 @@
   </si>
   <si>
     <t>Import</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -3499,7 +3502,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z81"/>
+  <dimension ref="A1:Z185"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
@@ -8225,6 +8228,4830 @@
         <v>38.9</v>
       </c>
     </row>
+    <row r="84" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A84" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="85" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A85" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="86" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A86" t="s">
+        <v>83</v>
+      </c>
+      <c r="B86">
+        <v>5802.1</v>
+      </c>
+      <c r="C86">
+        <v>5728.57</v>
+      </c>
+      <c r="D86">
+        <v>5846.23</v>
+      </c>
+      <c r="E86">
+        <v>5871.94</v>
+      </c>
+      <c r="F86">
+        <v>5955.9500000000007</v>
+      </c>
+      <c r="G86">
+        <v>6039.9900000000007</v>
+      </c>
+      <c r="H86">
+        <v>6052.94</v>
+      </c>
+      <c r="I86">
+        <v>6149.5699999999988</v>
+      </c>
+      <c r="J86">
+        <v>6115.5299999999988</v>
+      </c>
+      <c r="K86">
+        <v>5948.8200000000006</v>
+      </c>
+      <c r="L86">
+        <v>6123.94</v>
+      </c>
+      <c r="M86">
+        <v>6099.8700000000008</v>
+      </c>
+      <c r="N86">
+        <v>6052.67</v>
+      </c>
+      <c r="O86">
+        <v>6068.61</v>
+      </c>
+      <c r="P86">
+        <v>6110.0099999999993</v>
+      </c>
+      <c r="Q86">
+        <v>6098.99</v>
+      </c>
+      <c r="R86">
+        <v>6103.56</v>
+      </c>
+      <c r="S86">
+        <v>6069.3099999999995</v>
+      </c>
+      <c r="T86">
+        <v>6219.55</v>
+      </c>
+      <c r="U86">
+        <v>6177.3799999999992</v>
+      </c>
+      <c r="V86">
+        <v>6063.18</v>
+      </c>
+      <c r="W86">
+        <v>6174.62</v>
+      </c>
+      <c r="X86">
+        <v>6308.89</v>
+      </c>
+      <c r="Y86">
+        <v>6276.91</v>
+      </c>
+      <c r="Z86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A87" t="s">
+        <v>38</v>
+      </c>
+      <c r="B87">
+        <v>2000</v>
+      </c>
+      <c r="C87">
+        <v>2001</v>
+      </c>
+      <c r="D87">
+        <v>2002</v>
+      </c>
+      <c r="E87">
+        <v>2003</v>
+      </c>
+      <c r="F87">
+        <v>2004</v>
+      </c>
+      <c r="G87">
+        <v>2005</v>
+      </c>
+      <c r="H87">
+        <v>2006</v>
+      </c>
+      <c r="I87">
+        <v>2007</v>
+      </c>
+      <c r="J87">
+        <v>2008</v>
+      </c>
+      <c r="K87">
+        <v>2009</v>
+      </c>
+      <c r="L87">
+        <v>2010</v>
+      </c>
+      <c r="M87">
+        <v>2011</v>
+      </c>
+      <c r="N87">
+        <v>2012</v>
+      </c>
+      <c r="O87">
+        <v>2013</v>
+      </c>
+      <c r="P87">
+        <v>2014</v>
+      </c>
+      <c r="Q87">
+        <v>2015</v>
+      </c>
+      <c r="R87">
+        <v>2016</v>
+      </c>
+      <c r="S87">
+        <v>2017</v>
+      </c>
+      <c r="T87">
+        <v>2018</v>
+      </c>
+      <c r="U87">
+        <v>2019</v>
+      </c>
+      <c r="V87">
+        <v>2020</v>
+      </c>
+      <c r="W87">
+        <v>2021</v>
+      </c>
+      <c r="X87">
+        <v>2022</v>
+      </c>
+      <c r="Y87">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="88" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A88" t="s">
+        <v>31</v>
+      </c>
+      <c r="B88">
+        <v>74.819999999999993</v>
+      </c>
+      <c r="C88">
+        <v>64.64</v>
+      </c>
+      <c r="D88">
+        <v>69.849999999999994</v>
+      </c>
+      <c r="E88">
+        <v>70.19</v>
+      </c>
+      <c r="F88">
+        <v>70.489999999999995</v>
+      </c>
+      <c r="G88">
+        <v>70.92</v>
+      </c>
+      <c r="H88">
+        <v>71.37</v>
+      </c>
+      <c r="I88">
+        <v>72.239999999999995</v>
+      </c>
+      <c r="J88">
+        <v>72.349999999999994</v>
+      </c>
+      <c r="K88">
+        <v>71.960000000000008</v>
+      </c>
+      <c r="L88">
+        <v>73.92</v>
+      </c>
+      <c r="M88">
+        <v>74.81</v>
+      </c>
+      <c r="N88">
+        <v>75.88</v>
+      </c>
+      <c r="O88">
+        <v>79.62</v>
+      </c>
+      <c r="P88">
+        <v>83.07</v>
+      </c>
+      <c r="Q88">
+        <v>82.75</v>
+      </c>
+      <c r="R88">
+        <v>81.92</v>
+      </c>
+      <c r="S88">
+        <v>81.77</v>
+      </c>
+      <c r="T88">
+        <v>80.52</v>
+      </c>
+      <c r="U88">
+        <v>75.38</v>
+      </c>
+      <c r="V88">
+        <v>72.790000000000006</v>
+      </c>
+      <c r="W88">
+        <v>72.489999999999995</v>
+      </c>
+      <c r="X88">
+        <v>70.010000000000005</v>
+      </c>
+      <c r="Y88">
+        <v>65.650000000000006</v>
+      </c>
+    </row>
+    <row r="89" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A89" t="s">
+        <v>33</v>
+      </c>
+      <c r="B89">
+        <v>1966.27</v>
+      </c>
+      <c r="C89">
+        <v>1903.96</v>
+      </c>
+      <c r="D89">
+        <v>1933.13</v>
+      </c>
+      <c r="E89">
+        <v>1973.74</v>
+      </c>
+      <c r="F89">
+        <v>1978.3</v>
+      </c>
+      <c r="G89">
+        <v>2012.87</v>
+      </c>
+      <c r="H89">
+        <v>1990.51</v>
+      </c>
+      <c r="I89">
+        <v>2016.46</v>
+      </c>
+      <c r="J89">
+        <v>1985.8</v>
+      </c>
+      <c r="K89">
+        <v>1755.9</v>
+      </c>
+      <c r="L89">
+        <v>1847.29</v>
+      </c>
+      <c r="M89">
+        <v>1733.43</v>
+      </c>
+      <c r="N89">
+        <v>1514.04</v>
+      </c>
+      <c r="O89">
+        <v>1581.11</v>
+      </c>
+      <c r="P89">
+        <v>1581.71</v>
+      </c>
+      <c r="Q89">
+        <v>1352.4</v>
+      </c>
+      <c r="R89">
+        <v>1239.1500000000001</v>
+      </c>
+      <c r="S89">
+        <v>1205.8399999999999</v>
+      </c>
+      <c r="T89">
+        <v>1149.49</v>
+      </c>
+      <c r="U89">
+        <v>964.96</v>
+      </c>
+      <c r="V89">
+        <v>773.39</v>
+      </c>
+      <c r="W89">
+        <v>898</v>
+      </c>
+      <c r="X89">
+        <v>831.51</v>
+      </c>
+      <c r="Y89">
+        <v>675.11</v>
+      </c>
+    </row>
+    <row r="90" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A90" t="s">
+        <v>35</v>
+      </c>
+      <c r="B90">
+        <v>614.99</v>
+      </c>
+      <c r="C90">
+        <v>639.13</v>
+      </c>
+      <c r="D90">
+        <v>691.01</v>
+      </c>
+      <c r="E90">
+        <v>649.91</v>
+      </c>
+      <c r="F90">
+        <v>710.1</v>
+      </c>
+      <c r="G90">
+        <v>760.96</v>
+      </c>
+      <c r="H90">
+        <v>816.44</v>
+      </c>
+      <c r="I90">
+        <v>896.59</v>
+      </c>
+      <c r="J90">
+        <v>882.98</v>
+      </c>
+      <c r="K90">
+        <v>920.98</v>
+      </c>
+      <c r="L90">
+        <v>987.7</v>
+      </c>
+      <c r="M90">
+        <v>1013.69</v>
+      </c>
+      <c r="N90">
+        <v>1225.8900000000001</v>
+      </c>
+      <c r="O90">
+        <v>1124.8399999999999</v>
+      </c>
+      <c r="P90">
+        <v>1126.6099999999999</v>
+      </c>
+      <c r="Q90">
+        <v>1333.48</v>
+      </c>
+      <c r="R90">
+        <v>1378.31</v>
+      </c>
+      <c r="S90">
+        <v>1296.44</v>
+      </c>
+      <c r="T90">
+        <v>1469.13</v>
+      </c>
+      <c r="U90">
+        <v>1585.81</v>
+      </c>
+      <c r="V90">
+        <v>1624.17</v>
+      </c>
+      <c r="W90">
+        <v>1579.19</v>
+      </c>
+      <c r="X90">
+        <v>1687.06</v>
+      </c>
+      <c r="Y90">
+        <v>1806.06</v>
+      </c>
+    </row>
+    <row r="91" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A91" t="s">
+        <v>40</v>
+      </c>
+      <c r="B91">
+        <v>270.02999999999997</v>
+      </c>
+      <c r="C91">
+        <v>208.14</v>
+      </c>
+      <c r="D91">
+        <v>255.59</v>
+      </c>
+      <c r="E91">
+        <v>267.27</v>
+      </c>
+      <c r="F91">
+        <v>259.93</v>
+      </c>
+      <c r="G91">
+        <v>263.76</v>
+      </c>
+      <c r="H91">
+        <v>282.69</v>
+      </c>
+      <c r="I91">
+        <v>240.61</v>
+      </c>
+      <c r="J91">
+        <v>248.54</v>
+      </c>
+      <c r="K91">
+        <v>268.82</v>
+      </c>
+      <c r="L91">
+        <v>254.7</v>
+      </c>
+      <c r="M91">
+        <v>312.93</v>
+      </c>
+      <c r="N91">
+        <v>271.29000000000002</v>
+      </c>
+      <c r="O91">
+        <v>263.88</v>
+      </c>
+      <c r="P91">
+        <v>253.19</v>
+      </c>
+      <c r="Q91">
+        <v>243.99</v>
+      </c>
+      <c r="R91">
+        <v>261.13</v>
+      </c>
+      <c r="S91">
+        <v>293.83999999999997</v>
+      </c>
+      <c r="T91">
+        <v>286.62</v>
+      </c>
+      <c r="U91">
+        <v>282.61</v>
+      </c>
+      <c r="V91">
+        <v>279.95</v>
+      </c>
+      <c r="W91">
+        <v>246.47</v>
+      </c>
+      <c r="X91">
+        <v>248.76</v>
+      </c>
+      <c r="Y91">
+        <v>239.01</v>
+      </c>
+    </row>
+    <row r="92" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A92" t="s">
+        <v>41</v>
+      </c>
+      <c r="B92">
+        <v>753.89</v>
+      </c>
+      <c r="C92">
+        <v>768.83</v>
+      </c>
+      <c r="D92">
+        <v>780.06</v>
+      </c>
+      <c r="E92">
+        <v>763.73</v>
+      </c>
+      <c r="F92">
+        <v>788.53</v>
+      </c>
+      <c r="G92">
+        <v>781.99</v>
+      </c>
+      <c r="H92">
+        <v>787.22</v>
+      </c>
+      <c r="I92">
+        <v>806.42</v>
+      </c>
+      <c r="J92">
+        <v>806.21</v>
+      </c>
+      <c r="K92">
+        <v>798.85</v>
+      </c>
+      <c r="L92">
+        <v>806.97</v>
+      </c>
+      <c r="M92">
+        <v>790.2</v>
+      </c>
+      <c r="N92">
+        <v>769.33</v>
+      </c>
+      <c r="O92">
+        <v>789.02</v>
+      </c>
+      <c r="P92">
+        <v>797.17</v>
+      </c>
+      <c r="Q92">
+        <v>797.18</v>
+      </c>
+      <c r="R92">
+        <v>805.69</v>
+      </c>
+      <c r="S92">
+        <v>804.95</v>
+      </c>
+      <c r="T92">
+        <v>807.08</v>
+      </c>
+      <c r="U92">
+        <v>809.41</v>
+      </c>
+      <c r="V92">
+        <v>789.88</v>
+      </c>
+      <c r="W92">
+        <v>779.65</v>
+      </c>
+      <c r="X92">
+        <v>771.54</v>
+      </c>
+      <c r="Y92">
+        <v>774.87</v>
+      </c>
+    </row>
+    <row r="93" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A93" t="s">
+        <v>37</v>
+      </c>
+      <c r="B93">
+        <v>116.02</v>
+      </c>
+      <c r="C93">
+        <v>135.59</v>
+      </c>
+      <c r="D93">
+        <v>103.69</v>
+      </c>
+      <c r="E93">
+        <v>132.38</v>
+      </c>
+      <c r="F93">
+        <v>129.88</v>
+      </c>
+      <c r="G93">
+        <v>126.13</v>
+      </c>
+      <c r="H93">
+        <v>71.61</v>
+      </c>
+      <c r="I93">
+        <v>75.19</v>
+      </c>
+      <c r="J93">
+        <v>55.43</v>
+      </c>
+      <c r="K93">
+        <v>48.53</v>
+      </c>
+      <c r="L93">
+        <v>47.5</v>
+      </c>
+      <c r="M93">
+        <v>41.81</v>
+      </c>
+      <c r="N93">
+        <v>39.090000000000003</v>
+      </c>
+      <c r="O93">
+        <v>40.26</v>
+      </c>
+      <c r="P93">
+        <v>43.69</v>
+      </c>
+      <c r="Q93">
+        <v>44.44</v>
+      </c>
+      <c r="R93">
+        <v>39.5</v>
+      </c>
+      <c r="S93">
+        <v>37.89</v>
+      </c>
+      <c r="T93">
+        <v>42.68</v>
+      </c>
+      <c r="U93">
+        <v>37.44</v>
+      </c>
+      <c r="V93">
+        <v>34.340000000000003</v>
+      </c>
+      <c r="W93">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="X93">
+        <v>38.64</v>
+      </c>
+      <c r="Y93">
+        <v>33.130000000000003</v>
+      </c>
+    </row>
+    <row r="94" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A94" t="s">
+        <v>42</v>
+      </c>
+      <c r="B94">
+        <v>0.49</v>
+      </c>
+      <c r="C94">
+        <v>0.54</v>
+      </c>
+      <c r="D94">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E94">
+        <v>0.53</v>
+      </c>
+      <c r="F94">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="G94">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H94">
+        <v>0.51</v>
+      </c>
+      <c r="I94">
+        <v>0.61</v>
+      </c>
+      <c r="J94">
+        <v>0.86</v>
+      </c>
+      <c r="K94">
+        <v>0.89</v>
+      </c>
+      <c r="L94">
+        <v>1.21</v>
+      </c>
+      <c r="M94">
+        <v>1.82</v>
+      </c>
+      <c r="N94">
+        <v>4.33</v>
+      </c>
+      <c r="O94">
+        <v>9.0399999999999991</v>
+      </c>
+      <c r="P94">
+        <v>28.92</v>
+      </c>
+      <c r="Q94">
+        <v>39.03</v>
+      </c>
+      <c r="R94">
+        <v>54.87</v>
+      </c>
+      <c r="S94">
+        <v>77.28</v>
+      </c>
+      <c r="T94">
+        <v>93.36</v>
+      </c>
+      <c r="U94">
+        <v>106.89</v>
+      </c>
+      <c r="V94">
+        <v>130.72</v>
+      </c>
+      <c r="W94">
+        <v>164.42</v>
+      </c>
+      <c r="X94">
+        <v>205.07</v>
+      </c>
+      <c r="Y94">
+        <v>238.94</v>
+      </c>
+    </row>
+    <row r="95" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A95" t="s">
+        <v>43</v>
+      </c>
+      <c r="B95">
+        <v>5.59</v>
+      </c>
+      <c r="C95">
+        <v>6.74</v>
+      </c>
+      <c r="D95">
+        <v>10.35</v>
+      </c>
+      <c r="E95">
+        <v>11.19</v>
+      </c>
+      <c r="F95">
+        <v>14.14</v>
+      </c>
+      <c r="G95">
+        <v>17.809999999999999</v>
+      </c>
+      <c r="H95">
+        <v>26.59</v>
+      </c>
+      <c r="I95">
+        <v>34.450000000000003</v>
+      </c>
+      <c r="J95">
+        <v>55.36</v>
+      </c>
+      <c r="K95">
+        <v>73.89</v>
+      </c>
+      <c r="L95">
+        <v>94.65</v>
+      </c>
+      <c r="M95">
+        <v>120.18</v>
+      </c>
+      <c r="N95">
+        <v>140.82</v>
+      </c>
+      <c r="O95">
+        <v>167.84</v>
+      </c>
+      <c r="P95">
+        <v>181.65</v>
+      </c>
+      <c r="Q95">
+        <v>190.72</v>
+      </c>
+      <c r="R95">
+        <v>226.99</v>
+      </c>
+      <c r="S95">
+        <v>254.3</v>
+      </c>
+      <c r="T95">
+        <v>272.67</v>
+      </c>
+      <c r="U95">
+        <v>295.88</v>
+      </c>
+      <c r="V95">
+        <v>337.94</v>
+      </c>
+      <c r="W95">
+        <v>378.2</v>
+      </c>
+      <c r="X95">
+        <v>434.3</v>
+      </c>
+      <c r="Y95">
+        <v>421.14</v>
+      </c>
+    </row>
+    <row r="101" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A101" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="102" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A102" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="103" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A103" t="s">
+        <v>83</v>
+      </c>
+      <c r="B103">
+        <v>6052.6670009999998</v>
+      </c>
+      <c r="C103">
+        <v>7929.6069989999996</v>
+      </c>
+      <c r="D103">
+        <v>8108.2679980000003</v>
+      </c>
+      <c r="E103">
+        <v>8136.078998</v>
+      </c>
+      <c r="F103">
+        <v>8235.913000999999</v>
+      </c>
+      <c r="G103">
+        <v>8360.4679980000019</v>
+      </c>
+      <c r="H103">
+        <v>8376.1310000000012</v>
+      </c>
+      <c r="I103">
+        <v>8429.8409979999997</v>
+      </c>
+      <c r="J103">
+        <v>8454.7620009999991</v>
+      </c>
+      <c r="K103">
+        <v>8286.4149980000002</v>
+      </c>
+      <c r="L103">
+        <v>8467.729999000001</v>
+      </c>
+      <c r="M103">
+        <v>8434.6630000000005</v>
+      </c>
+      <c r="N103">
+        <v>8380.9599989999988</v>
+      </c>
+      <c r="O103">
+        <v>8402.6710009999988</v>
+      </c>
+      <c r="P103">
+        <v>8449.1710019999991</v>
+      </c>
+      <c r="Q103">
+        <v>8425.9589969999979</v>
+      </c>
+      <c r="R103">
+        <v>8437.9379979999994</v>
+      </c>
+      <c r="S103">
+        <v>8398.3230040000017</v>
+      </c>
+      <c r="T103">
+        <v>8565.5390000000007</v>
+      </c>
+      <c r="U103">
+        <v>8500.8639989999974</v>
+      </c>
+      <c r="V103">
+        <v>8378.1440009999988</v>
+      </c>
+      <c r="W103">
+        <v>8491.1780020000024</v>
+      </c>
+      <c r="X103">
+        <v>8605.469000000001</v>
+      </c>
+      <c r="Y103">
+        <v>2094.8000000000002</v>
+      </c>
+      <c r="Z103">
+        <v>2081.8000000000002</v>
+      </c>
+    </row>
+    <row r="104" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A104" t="s">
+        <v>38</v>
+      </c>
+      <c r="B104">
+        <v>2000</v>
+      </c>
+      <c r="C104">
+        <v>2001</v>
+      </c>
+      <c r="D104">
+        <v>2002</v>
+      </c>
+      <c r="E104">
+        <v>2003</v>
+      </c>
+      <c r="F104">
+        <v>2004</v>
+      </c>
+      <c r="G104">
+        <v>2005</v>
+      </c>
+      <c r="H104">
+        <v>2006</v>
+      </c>
+      <c r="I104">
+        <v>2007</v>
+      </c>
+      <c r="J104">
+        <v>2008</v>
+      </c>
+      <c r="K104">
+        <v>2009</v>
+      </c>
+      <c r="L104">
+        <v>2010</v>
+      </c>
+      <c r="M104">
+        <v>2011</v>
+      </c>
+      <c r="N104">
+        <v>2012</v>
+      </c>
+      <c r="O104">
+        <v>2013</v>
+      </c>
+      <c r="P104">
+        <v>2014</v>
+      </c>
+      <c r="Q104">
+        <v>2015</v>
+      </c>
+      <c r="R104">
+        <v>2016</v>
+      </c>
+      <c r="S104">
+        <v>2017</v>
+      </c>
+      <c r="T104">
+        <v>2018</v>
+      </c>
+      <c r="U104">
+        <v>2019</v>
+      </c>
+      <c r="V104">
+        <v>2020</v>
+      </c>
+      <c r="W104">
+        <v>2021</v>
+      </c>
+      <c r="X104">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="105" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A105" t="s">
+        <v>31</v>
+      </c>
+      <c r="B105">
+        <v>56.180000999999997</v>
+      </c>
+      <c r="C105">
+        <v>50.336998999999999</v>
+      </c>
+      <c r="D105">
+        <v>54.022998000000001</v>
+      </c>
+      <c r="E105">
+        <v>54.120998</v>
+      </c>
+      <c r="F105">
+        <v>55.783000999999999</v>
+      </c>
+      <c r="G105">
+        <v>57.980998000000007</v>
+      </c>
+      <c r="H105">
+        <v>58.795999999999999</v>
+      </c>
+      <c r="I105">
+        <v>59.120998</v>
+      </c>
+      <c r="J105">
+        <v>59.647000999999996</v>
+      </c>
+      <c r="K105">
+        <v>59.318998000000001</v>
+      </c>
+      <c r="L105">
+        <v>61.743999000000002</v>
+      </c>
+      <c r="M105">
+        <v>62.319999999999993</v>
+      </c>
+      <c r="N105">
+        <v>64.108999000000011</v>
+      </c>
+      <c r="O105">
+        <v>66.93900099999999</v>
+      </c>
+      <c r="P105">
+        <v>70.818002000000007</v>
+      </c>
+      <c r="Q105">
+        <v>70.066997000000001</v>
+      </c>
+      <c r="R105">
+        <v>69.016998000000001</v>
+      </c>
+      <c r="S105">
+        <v>68.857004000000003</v>
+      </c>
+      <c r="T105">
+        <v>67.885000000000005</v>
+      </c>
+      <c r="U105">
+        <v>63.193999000000005</v>
+      </c>
+      <c r="V105">
+        <v>60.269001000000003</v>
+      </c>
+      <c r="W105">
+        <v>59.582001999999996</v>
+      </c>
+      <c r="X105">
+        <v>57.146000000000001</v>
+      </c>
+    </row>
+    <row r="106" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A106" t="s">
+        <v>33</v>
+      </c>
+      <c r="B106">
+        <v>2129.498</v>
+      </c>
+      <c r="C106">
+        <v>1982.12</v>
+      </c>
+      <c r="D106">
+        <v>2039.665</v>
+      </c>
+      <c r="E106">
+        <v>2083.326</v>
+      </c>
+      <c r="F106">
+        <v>2090.4949999999999</v>
+      </c>
+      <c r="G106">
+        <v>2153.9560000000001</v>
+      </c>
+      <c r="H106">
+        <v>2127.7959999999998</v>
+      </c>
+      <c r="I106">
+        <v>2118.4549999999999</v>
+      </c>
+      <c r="J106">
+        <v>2132.596</v>
+      </c>
+      <c r="K106">
+        <v>1892.6610000000001</v>
+      </c>
+      <c r="L106">
+        <v>1994.194</v>
+      </c>
+      <c r="M106">
+        <v>1875.413</v>
+      </c>
+      <c r="N106">
+        <v>1643.43</v>
+      </c>
+      <c r="O106">
+        <v>1712.4079999999999</v>
+      </c>
+      <c r="P106">
+        <v>1712.577</v>
+      </c>
+      <c r="Q106">
+        <v>1470.9970000000001</v>
+      </c>
+      <c r="R106">
+        <v>1354.0340000000001</v>
+      </c>
+      <c r="S106">
+        <v>1321.4190000000001</v>
+      </c>
+      <c r="T106">
+        <v>1272.1500000000001</v>
+      </c>
+      <c r="U106">
+        <v>1069.528</v>
+      </c>
+      <c r="V106">
+        <v>855.77</v>
+      </c>
+      <c r="W106">
+        <v>991.56100000000004</v>
+      </c>
+      <c r="X106">
+        <v>913.30200000000002</v>
+      </c>
+    </row>
+    <row r="107" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A107" t="s">
+        <v>35</v>
+      </c>
+      <c r="B107">
+        <v>634.29</v>
+      </c>
+      <c r="C107">
+        <v>659.91399999999999</v>
+      </c>
+      <c r="D107">
+        <v>712.43200000000002</v>
+      </c>
+      <c r="E107">
+        <v>670.19200000000001</v>
+      </c>
+      <c r="F107">
+        <v>731.55200000000002</v>
+      </c>
+      <c r="G107">
+        <v>782.82899999999995</v>
+      </c>
+      <c r="H107">
+        <v>842.774</v>
+      </c>
+      <c r="I107">
+        <v>915.19600000000003</v>
+      </c>
+      <c r="J107">
+        <v>910.17600000000004</v>
+      </c>
+      <c r="K107">
+        <v>949.77599999999995</v>
+      </c>
+      <c r="L107">
+        <v>1017.869</v>
+      </c>
+      <c r="M107">
+        <v>1045.2539999999999</v>
+      </c>
+      <c r="N107">
+        <v>1264.5519999999999</v>
+      </c>
+      <c r="O107">
+        <v>1158.454</v>
+      </c>
+      <c r="P107">
+        <v>1161.3330000000001</v>
+      </c>
+      <c r="Q107">
+        <v>1372.57</v>
+      </c>
+      <c r="R107">
+        <v>1418.1</v>
+      </c>
+      <c r="S107">
+        <v>1337.703</v>
+      </c>
+      <c r="T107">
+        <v>1519.2170000000001</v>
+      </c>
+      <c r="U107">
+        <v>1639.826</v>
+      </c>
+      <c r="V107">
+        <v>1680.143</v>
+      </c>
+      <c r="W107">
+        <v>1634.0889999999999</v>
+      </c>
+      <c r="X107">
+        <v>1740.421</v>
+      </c>
+    </row>
+    <row r="108" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A108" t="s">
+        <v>39</v>
+      </c>
+      <c r="B108">
+        <v>14.621</v>
+      </c>
+      <c r="C108">
+        <v>14.246</v>
+      </c>
+      <c r="D108">
+        <v>14.939</v>
+      </c>
+      <c r="E108">
+        <v>14.87</v>
+      </c>
+      <c r="F108">
+        <v>15.487</v>
+      </c>
+      <c r="G108">
+        <v>16.777999999999999</v>
+      </c>
+      <c r="H108">
+        <v>16.581</v>
+      </c>
+      <c r="I108">
+        <v>16.797999999999998</v>
+      </c>
+      <c r="J108">
+        <v>16.873000000000001</v>
+      </c>
+      <c r="K108">
+        <v>17.045999999999999</v>
+      </c>
+      <c r="L108">
+        <v>17.577000000000002</v>
+      </c>
+      <c r="M108">
+        <v>17.84</v>
+      </c>
+      <c r="N108">
+        <v>18.135000000000002</v>
+      </c>
+      <c r="O108">
+        <v>18.422000000000001</v>
+      </c>
+      <c r="P108">
+        <v>18.71</v>
+      </c>
+      <c r="Q108">
+        <v>18.727</v>
+      </c>
+      <c r="R108">
+        <v>18.584</v>
+      </c>
+      <c r="S108">
+        <v>18.725999999999999</v>
+      </c>
+      <c r="T108">
+        <v>18.773</v>
+      </c>
+      <c r="U108">
+        <v>18.364000000000001</v>
+      </c>
+      <c r="V108">
+        <v>18.831</v>
+      </c>
+      <c r="W108">
+        <v>19.077000000000002</v>
+      </c>
+      <c r="X108">
+        <v>19.141999999999999</v>
+      </c>
+    </row>
+    <row r="109" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A109" t="s">
+        <v>40</v>
+      </c>
+      <c r="B109">
+        <v>279.98599999999999</v>
+      </c>
+      <c r="C109">
+        <v>214.72800000000001</v>
+      </c>
+      <c r="D109">
+        <v>291.755</v>
+      </c>
+      <c r="E109">
+        <v>305.72399999999999</v>
+      </c>
+      <c r="F109">
+        <v>297.89400000000001</v>
+      </c>
+      <c r="G109">
+        <v>297.92599999999999</v>
+      </c>
+      <c r="H109">
+        <v>317.68900000000002</v>
+      </c>
+      <c r="I109">
+        <v>275.54500000000002</v>
+      </c>
+      <c r="J109">
+        <v>281.995</v>
+      </c>
+      <c r="K109">
+        <v>298.40999999999997</v>
+      </c>
+      <c r="L109">
+        <v>286.33300000000003</v>
+      </c>
+      <c r="M109">
+        <v>344.56099999999998</v>
+      </c>
+      <c r="N109">
+        <v>298.28700000000003</v>
+      </c>
+      <c r="O109">
+        <v>290.113</v>
+      </c>
+      <c r="P109">
+        <v>281.52699999999999</v>
+      </c>
+      <c r="Q109">
+        <v>271.12900000000002</v>
+      </c>
+      <c r="R109">
+        <v>292.113</v>
+      </c>
+      <c r="S109">
+        <v>325.11400000000003</v>
+      </c>
+      <c r="T109">
+        <v>317.00399999999996</v>
+      </c>
+      <c r="U109">
+        <v>310.57099999999997</v>
+      </c>
+      <c r="V109">
+        <v>308.21299999999997</v>
+      </c>
+      <c r="W109">
+        <v>274.096</v>
+      </c>
+      <c r="X109">
+        <v>279.06799999999998</v>
+      </c>
+    </row>
+    <row r="110" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A110" t="s">
+        <v>41</v>
+      </c>
+      <c r="B110">
+        <v>797.71799999999996</v>
+      </c>
+      <c r="C110">
+        <v>792.60400000000004</v>
+      </c>
+      <c r="D110">
+        <v>804.51900000000001</v>
+      </c>
+      <c r="E110">
+        <v>787.81799999999998</v>
+      </c>
+      <c r="F110">
+        <v>813.33900000000006</v>
+      </c>
+      <c r="G110">
+        <v>810.726</v>
+      </c>
+      <c r="H110">
+        <v>816.19500000000005</v>
+      </c>
+      <c r="I110">
+        <v>836.63400000000001</v>
+      </c>
+      <c r="J110">
+        <v>837.80399999999997</v>
+      </c>
+      <c r="K110">
+        <v>830.21</v>
+      </c>
+      <c r="L110">
+        <v>838.93100000000004</v>
+      </c>
+      <c r="M110">
+        <v>821.40499999999997</v>
+      </c>
+      <c r="N110">
+        <v>801.12900000000002</v>
+      </c>
+      <c r="O110">
+        <v>822.00400000000002</v>
+      </c>
+      <c r="P110">
+        <v>830.58399999999995</v>
+      </c>
+      <c r="Q110">
+        <v>830.28800000000001</v>
+      </c>
+      <c r="R110">
+        <v>839.91800000000001</v>
+      </c>
+      <c r="S110">
+        <v>838.86099999999999</v>
+      </c>
+      <c r="T110">
+        <v>841.32899999999995</v>
+      </c>
+      <c r="U110">
+        <v>843.33</v>
+      </c>
+      <c r="V110">
+        <v>823.15</v>
+      </c>
+      <c r="W110">
+        <v>811.55100000000004</v>
+      </c>
+      <c r="X110">
+        <v>803.66899999999998</v>
+      </c>
+    </row>
+    <row r="111" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A111" t="s">
+        <v>37</v>
+      </c>
+      <c r="B111">
+        <v>134.01499999999999</v>
+      </c>
+      <c r="C111">
+        <v>143.767</v>
+      </c>
+      <c r="D111">
+        <v>121.646</v>
+      </c>
+      <c r="E111">
+        <v>152.88</v>
+      </c>
+      <c r="F111">
+        <v>154.70699999999999</v>
+      </c>
+      <c r="G111">
+        <v>155.17099999999999</v>
+      </c>
+      <c r="H111">
+        <v>93.036999999999992</v>
+      </c>
+      <c r="I111">
+        <v>91.814999999999998</v>
+      </c>
+      <c r="J111">
+        <v>71.382000000000005</v>
+      </c>
+      <c r="K111">
+        <v>64.051999999999992</v>
+      </c>
+      <c r="L111">
+        <v>62.692</v>
+      </c>
+      <c r="M111">
+        <v>55.600999999999999</v>
+      </c>
+      <c r="N111">
+        <v>48.951000000000001</v>
+      </c>
+      <c r="O111">
+        <v>52.445999999999998</v>
+      </c>
+      <c r="P111">
+        <v>55.166000000000004</v>
+      </c>
+      <c r="Q111">
+        <v>54.754000000000005</v>
+      </c>
+      <c r="R111">
+        <v>50.466999999999999</v>
+      </c>
+      <c r="S111">
+        <v>47.513999999999996</v>
+      </c>
+      <c r="T111">
+        <v>58.063000000000002</v>
+      </c>
+      <c r="U111">
+        <v>51.272999999999996</v>
+      </c>
+      <c r="V111">
+        <v>52.521000000000001</v>
+      </c>
+      <c r="W111">
+        <v>50.584999999999994</v>
+      </c>
+      <c r="X111">
+        <v>56.28</v>
+      </c>
+    </row>
+    <row r="112" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A112" t="s">
+        <v>42</v>
+      </c>
+      <c r="B112">
+        <v>0.70900000000000007</v>
+      </c>
+      <c r="C112">
+        <v>0.78499999999999992</v>
+      </c>
+      <c r="D112">
+        <v>0.83</v>
+      </c>
+      <c r="E112">
+        <v>0.84800000000000009</v>
+      </c>
+      <c r="F112">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="G112">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="H112">
+        <v>1.2869999999999999</v>
+      </c>
+      <c r="I112">
+        <v>1.6739999999999999</v>
+      </c>
+      <c r="J112">
+        <v>2.093</v>
+      </c>
+      <c r="K112">
+        <v>2.5150000000000001</v>
+      </c>
+      <c r="L112">
+        <v>3.9420000000000002</v>
+      </c>
+      <c r="M112">
+        <v>6.2149999999999999</v>
+      </c>
+      <c r="N112">
+        <v>10.145</v>
+      </c>
+      <c r="O112">
+        <v>15.872</v>
+      </c>
+      <c r="P112">
+        <v>25.763999999999999</v>
+      </c>
+      <c r="Q112">
+        <v>35.634999999999998</v>
+      </c>
+      <c r="R112">
+        <v>50.334000000000003</v>
+      </c>
+      <c r="S112">
+        <v>70.98</v>
+      </c>
+      <c r="T112">
+        <v>85.183999999999997</v>
+      </c>
+      <c r="U112">
+        <v>97.477999999999994</v>
+      </c>
+      <c r="V112">
+        <v>119.32900000000001</v>
+      </c>
+      <c r="W112">
+        <v>151.32299999999998</v>
+      </c>
+      <c r="X112">
+        <v>187.071</v>
+      </c>
+    </row>
+    <row r="113" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A113" t="s">
+        <v>43</v>
+      </c>
+      <c r="B113">
+        <v>5.65</v>
+      </c>
+      <c r="C113">
+        <v>6.806</v>
+      </c>
+      <c r="D113">
+        <v>10.459</v>
+      </c>
+      <c r="E113">
+        <v>11.3</v>
+      </c>
+      <c r="F113">
+        <v>14.291</v>
+      </c>
+      <c r="G113">
+        <v>17.881</v>
+      </c>
+      <c r="H113">
+        <v>26.675999999999998</v>
+      </c>
+      <c r="I113">
+        <v>34.603000000000002</v>
+      </c>
+      <c r="J113">
+        <v>55.695999999999998</v>
+      </c>
+      <c r="K113">
+        <v>74.225999999999999</v>
+      </c>
+      <c r="L113">
+        <v>95.147999999999996</v>
+      </c>
+      <c r="M113">
+        <v>120.854</v>
+      </c>
+      <c r="N113">
+        <v>141.922</v>
+      </c>
+      <c r="O113">
+        <v>169.71299999999999</v>
+      </c>
+      <c r="P113">
+        <v>183.892</v>
+      </c>
+      <c r="Q113">
+        <v>192.99200000000002</v>
+      </c>
+      <c r="R113">
+        <v>229.471</v>
+      </c>
+      <c r="S113">
+        <v>257.24900000000002</v>
+      </c>
+      <c r="T113">
+        <v>275.834</v>
+      </c>
+      <c r="U113">
+        <v>298.2</v>
+      </c>
+      <c r="V113">
+        <v>341.81799999999998</v>
+      </c>
+      <c r="W113">
+        <v>382.81400000000002</v>
+      </c>
+      <c r="X113">
+        <v>439.27</v>
+      </c>
+    </row>
+    <row r="116" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A116" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="117" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A117" t="s">
+        <v>80</v>
+      </c>
+      <c r="B117" t="s">
+        <v>10</v>
+      </c>
+      <c r="C117">
+        <v>2000</v>
+      </c>
+      <c r="D117">
+        <v>2001</v>
+      </c>
+      <c r="E117">
+        <v>2002</v>
+      </c>
+      <c r="F117">
+        <v>2003</v>
+      </c>
+      <c r="G117">
+        <v>2004</v>
+      </c>
+      <c r="H117">
+        <v>2005</v>
+      </c>
+      <c r="I117">
+        <v>2006</v>
+      </c>
+      <c r="J117">
+        <v>2007</v>
+      </c>
+      <c r="K117">
+        <v>2008</v>
+      </c>
+      <c r="L117">
+        <v>2009</v>
+      </c>
+      <c r="M117">
+        <v>2010</v>
+      </c>
+      <c r="N117">
+        <v>2011</v>
+      </c>
+      <c r="O117">
+        <v>2012</v>
+      </c>
+      <c r="P117">
+        <v>2013</v>
+      </c>
+      <c r="Q117">
+        <v>2014</v>
+      </c>
+      <c r="R117">
+        <v>2015</v>
+      </c>
+      <c r="S117">
+        <v>2016</v>
+      </c>
+      <c r="T117">
+        <v>2017</v>
+      </c>
+      <c r="U117">
+        <v>2018</v>
+      </c>
+      <c r="V117">
+        <v>2019</v>
+      </c>
+      <c r="W117">
+        <v>2020</v>
+      </c>
+      <c r="X117">
+        <v>2021</v>
+      </c>
+      <c r="Y117">
+        <v>2022</v>
+      </c>
+      <c r="Z117">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="118" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A118" t="s">
+        <v>47</v>
+      </c>
+      <c r="B118" t="s">
+        <v>81</v>
+      </c>
+      <c r="C118">
+        <v>14.7</v>
+      </c>
+      <c r="D118">
+        <v>16.5</v>
+      </c>
+      <c r="E118">
+        <v>13.6</v>
+      </c>
+      <c r="F118">
+        <v>24</v>
+      </c>
+      <c r="G118">
+        <v>22.9</v>
+      </c>
+      <c r="H118">
+        <v>19.8</v>
+      </c>
+      <c r="I118">
+        <v>24.3</v>
+      </c>
+      <c r="J118">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="K118">
+        <v>24.2</v>
+      </c>
+      <c r="L118">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="M118">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="N118">
+        <v>15</v>
+      </c>
+      <c r="O118">
+        <v>12</v>
+      </c>
+      <c r="P118">
+        <v>11.4</v>
+      </c>
+      <c r="Q118">
+        <v>13.3</v>
+      </c>
+      <c r="R118">
+        <v>9.1</v>
+      </c>
+      <c r="S118">
+        <v>6.2</v>
+      </c>
+      <c r="T118">
+        <v>9.4</v>
+      </c>
+      <c r="U118">
+        <v>13.8</v>
+      </c>
+      <c r="V118">
+        <v>20</v>
+      </c>
+      <c r="W118">
+        <v>14.1</v>
+      </c>
+      <c r="X118">
+        <v>13.9</v>
+      </c>
+      <c r="Y118">
+        <v>15.8</v>
+      </c>
+      <c r="Z118">
+        <v>19.899999999999999</v>
+      </c>
+    </row>
+    <row r="119" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A119" t="s">
+        <v>47</v>
+      </c>
+      <c r="B119" t="s">
+        <v>82</v>
+      </c>
+      <c r="C119">
+        <v>48.6</v>
+      </c>
+      <c r="D119">
+        <v>38.5</v>
+      </c>
+      <c r="E119">
+        <v>36.4</v>
+      </c>
+      <c r="F119">
+        <v>30.4</v>
+      </c>
+      <c r="G119">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="H119">
+        <v>44.5</v>
+      </c>
+      <c r="I119">
+        <v>42.7</v>
+      </c>
+      <c r="J119">
+        <v>51.4</v>
+      </c>
+      <c r="K119">
+        <v>57</v>
+      </c>
+      <c r="L119">
+        <v>52.2</v>
+      </c>
+      <c r="M119">
+        <v>45.1</v>
+      </c>
+      <c r="N119">
+        <v>52.3</v>
+      </c>
+      <c r="O119">
+        <v>59.3</v>
+      </c>
+      <c r="P119">
+        <v>70.400000000000006</v>
+      </c>
+      <c r="Q119">
+        <v>66.5</v>
+      </c>
+      <c r="R119">
+        <v>75.8</v>
+      </c>
+      <c r="S119">
+        <v>72.7</v>
+      </c>
+      <c r="T119">
+        <v>65.7</v>
+      </c>
+      <c r="U119">
+        <v>58.3</v>
+      </c>
+      <c r="V119">
+        <v>59.1</v>
+      </c>
+      <c r="W119">
+        <v>61.4</v>
+      </c>
+      <c r="X119">
+        <v>53.2</v>
+      </c>
+      <c r="Y119">
+        <v>57</v>
+      </c>
+      <c r="Z119">
+        <v>38.9</v>
+      </c>
+    </row>
+    <row r="123" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A123" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="124" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A124" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="125" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A125" t="s">
+        <v>38</v>
+      </c>
+      <c r="B125">
+        <v>2000</v>
+      </c>
+      <c r="C125">
+        <v>2001</v>
+      </c>
+      <c r="D125">
+        <v>2002</v>
+      </c>
+      <c r="E125">
+        <v>2003</v>
+      </c>
+      <c r="F125">
+        <v>2004</v>
+      </c>
+      <c r="G125">
+        <v>2005</v>
+      </c>
+      <c r="H125">
+        <v>2006</v>
+      </c>
+      <c r="I125">
+        <v>2007</v>
+      </c>
+      <c r="J125">
+        <v>2008</v>
+      </c>
+      <c r="K125">
+        <v>2009</v>
+      </c>
+      <c r="L125">
+        <v>2010</v>
+      </c>
+      <c r="M125">
+        <v>2011</v>
+      </c>
+      <c r="N125">
+        <v>2012</v>
+      </c>
+      <c r="O125">
+        <v>2013</v>
+      </c>
+      <c r="P125">
+        <v>2014</v>
+      </c>
+      <c r="Q125">
+        <v>2015</v>
+      </c>
+      <c r="R125">
+        <v>2016</v>
+      </c>
+      <c r="S125">
+        <v>2017</v>
+      </c>
+      <c r="T125">
+        <v>2018</v>
+      </c>
+      <c r="U125">
+        <v>2019</v>
+      </c>
+      <c r="V125">
+        <v>2020</v>
+      </c>
+      <c r="W125">
+        <v>2021</v>
+      </c>
+      <c r="X125">
+        <v>2022</v>
+      </c>
+      <c r="Y125">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="126" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A126" t="s">
+        <v>31</v>
+      </c>
+      <c r="B126">
+        <v>9.59</v>
+      </c>
+      <c r="C126">
+        <v>10.59</v>
+      </c>
+      <c r="D126">
+        <v>10.66</v>
+      </c>
+      <c r="E126">
+        <v>10.540000000000001</v>
+      </c>
+      <c r="F126">
+        <v>10.76</v>
+      </c>
+      <c r="G126">
+        <v>11</v>
+      </c>
+      <c r="H126">
+        <v>11.280000000000001</v>
+      </c>
+      <c r="I126">
+        <v>11.94</v>
+      </c>
+      <c r="J126">
+        <v>12.17</v>
+      </c>
+      <c r="K126">
+        <v>12.53</v>
+      </c>
+      <c r="L126">
+        <v>12.7</v>
+      </c>
+      <c r="M126">
+        <v>12.899999999999999</v>
+      </c>
+      <c r="N126">
+        <v>13.809999999999999</v>
+      </c>
+      <c r="O126">
+        <v>14.89</v>
+      </c>
+      <c r="P126">
+        <v>14.93</v>
+      </c>
+      <c r="Q126">
+        <v>15.52</v>
+      </c>
+      <c r="R126">
+        <v>15.42</v>
+      </c>
+      <c r="S126">
+        <v>15.33</v>
+      </c>
+      <c r="T126">
+        <v>15.06</v>
+      </c>
+      <c r="U126">
+        <v>14.61</v>
+      </c>
+      <c r="V126">
+        <v>14.46</v>
+      </c>
+      <c r="W126">
+        <v>13.94</v>
+      </c>
+      <c r="X126">
+        <v>13.75</v>
+      </c>
+      <c r="Y126">
+        <v>13.66</v>
+      </c>
+    </row>
+    <row r="127" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A127" t="s">
+        <v>33</v>
+      </c>
+      <c r="B127">
+        <v>334.24</v>
+      </c>
+      <c r="C127">
+        <v>335.32</v>
+      </c>
+      <c r="D127">
+        <v>335.8</v>
+      </c>
+      <c r="E127">
+        <v>334.47</v>
+      </c>
+      <c r="F127">
+        <v>334.48</v>
+      </c>
+      <c r="G127">
+        <v>334.63</v>
+      </c>
+      <c r="H127">
+        <v>334.94</v>
+      </c>
+      <c r="I127">
+        <v>333.64</v>
+      </c>
+      <c r="J127">
+        <v>334.56</v>
+      </c>
+      <c r="K127">
+        <v>335.94</v>
+      </c>
+      <c r="L127">
+        <v>339.36</v>
+      </c>
+      <c r="M127">
+        <v>340.2</v>
+      </c>
+      <c r="N127">
+        <v>332.88</v>
+      </c>
+      <c r="O127">
+        <v>327.89</v>
+      </c>
+      <c r="P127">
+        <v>323.38</v>
+      </c>
+      <c r="Q127">
+        <v>301.70999999999998</v>
+      </c>
+      <c r="R127">
+        <v>285.75</v>
+      </c>
+      <c r="S127">
+        <v>276.88</v>
+      </c>
+      <c r="T127">
+        <v>260.95</v>
+      </c>
+      <c r="U127">
+        <v>244.7</v>
+      </c>
+      <c r="V127">
+        <v>233.04</v>
+      </c>
+      <c r="W127">
+        <v>224.59</v>
+      </c>
+      <c r="X127">
+        <v>209.94</v>
+      </c>
+      <c r="Y127">
+        <v>200.28</v>
+      </c>
+    </row>
+    <row r="128" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A128" t="s">
+        <v>35</v>
+      </c>
+      <c r="B128">
+        <v>161.54</v>
+      </c>
+      <c r="C128">
+        <v>199.67</v>
+      </c>
+      <c r="D128">
+        <v>264.55</v>
+      </c>
+      <c r="E128">
+        <v>319.04000000000002</v>
+      </c>
+      <c r="F128">
+        <v>343.88</v>
+      </c>
+      <c r="G128">
+        <v>359.84</v>
+      </c>
+      <c r="H128">
+        <v>371.13</v>
+      </c>
+      <c r="I128">
+        <v>378.97</v>
+      </c>
+      <c r="J128">
+        <v>388.45</v>
+      </c>
+      <c r="K128">
+        <v>399.05</v>
+      </c>
+      <c r="L128">
+        <v>407.07</v>
+      </c>
+      <c r="M128">
+        <v>418.3</v>
+      </c>
+      <c r="N128">
+        <v>429.01</v>
+      </c>
+      <c r="O128">
+        <v>437.26</v>
+      </c>
+      <c r="P128">
+        <v>448.9</v>
+      </c>
+      <c r="Q128">
+        <v>460.37</v>
+      </c>
+      <c r="R128">
+        <v>473.01</v>
+      </c>
+      <c r="S128">
+        <v>484.89</v>
+      </c>
+      <c r="T128">
+        <v>509.07</v>
+      </c>
+      <c r="U128">
+        <v>519.28</v>
+      </c>
+      <c r="V128">
+        <v>523.75</v>
+      </c>
+      <c r="W128">
+        <v>530.26</v>
+      </c>
+      <c r="X128">
+        <v>535.49</v>
+      </c>
+      <c r="Y128">
+        <v>542.92999999999995</v>
+      </c>
+    </row>
+    <row r="129" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A129" t="s">
+        <v>40</v>
+      </c>
+      <c r="B129">
+        <v>79.36</v>
+      </c>
+      <c r="C129">
+        <v>78.92</v>
+      </c>
+      <c r="D129">
+        <v>79.36</v>
+      </c>
+      <c r="E129">
+        <v>78.69</v>
+      </c>
+      <c r="F129">
+        <v>77.64</v>
+      </c>
+      <c r="G129">
+        <v>77.540000000000006</v>
+      </c>
+      <c r="H129">
+        <v>77.819999999999993</v>
+      </c>
+      <c r="I129">
+        <v>77.88</v>
+      </c>
+      <c r="J129">
+        <v>77.930000000000007</v>
+      </c>
+      <c r="K129">
+        <v>78.52</v>
+      </c>
+      <c r="L129">
+        <v>82.61</v>
+      </c>
+      <c r="M129">
+        <v>82.45</v>
+      </c>
+      <c r="N129">
+        <v>82.56</v>
+      </c>
+      <c r="O129">
+        <v>83.01</v>
+      </c>
+      <c r="P129">
+        <v>83.49</v>
+      </c>
+      <c r="Q129">
+        <v>83.5</v>
+      </c>
+      <c r="R129">
+        <v>83.82</v>
+      </c>
+      <c r="S129">
+        <v>83.79</v>
+      </c>
+      <c r="T129">
+        <v>83.88</v>
+      </c>
+      <c r="U129">
+        <v>83.79</v>
+      </c>
+      <c r="V129">
+        <v>83.83</v>
+      </c>
+      <c r="W129">
+        <v>84.29</v>
+      </c>
+      <c r="X129">
+        <v>86.63</v>
+      </c>
+      <c r="Y129">
+        <v>86.66</v>
+      </c>
+    </row>
+    <row r="130" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A130" t="s">
+        <v>41</v>
+      </c>
+      <c r="B130">
+        <v>97.86</v>
+      </c>
+      <c r="C130">
+        <v>98.16</v>
+      </c>
+      <c r="D130">
+        <v>98.66</v>
+      </c>
+      <c r="E130">
+        <v>99.21</v>
+      </c>
+      <c r="F130">
+        <v>99.63</v>
+      </c>
+      <c r="G130">
+        <v>99.99</v>
+      </c>
+      <c r="H130">
+        <v>100.33</v>
+      </c>
+      <c r="I130">
+        <v>100.27</v>
+      </c>
+      <c r="J130">
+        <v>100.75</v>
+      </c>
+      <c r="K130">
+        <v>101</v>
+      </c>
+      <c r="L130">
+        <v>101.17</v>
+      </c>
+      <c r="M130">
+        <v>101.42</v>
+      </c>
+      <c r="N130">
+        <v>101.89</v>
+      </c>
+      <c r="O130">
+        <v>99.24</v>
+      </c>
+      <c r="P130">
+        <v>98.57</v>
+      </c>
+      <c r="Q130">
+        <v>98.67</v>
+      </c>
+      <c r="R130">
+        <v>99.56</v>
+      </c>
+      <c r="S130">
+        <v>99.63</v>
+      </c>
+      <c r="T130">
+        <v>99.43</v>
+      </c>
+      <c r="U130">
+        <v>98.12</v>
+      </c>
+      <c r="V130">
+        <v>96.5</v>
+      </c>
+      <c r="W130">
+        <v>95.55</v>
+      </c>
+      <c r="X130">
+        <v>94.66</v>
+      </c>
+      <c r="Y130">
+        <v>95.77</v>
+      </c>
+    </row>
+    <row r="131" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A131" t="s">
+        <v>37</v>
+      </c>
+      <c r="B131">
+        <v>86.09</v>
+      </c>
+      <c r="C131">
+        <v>87.75</v>
+      </c>
+      <c r="D131">
+        <v>61.52</v>
+      </c>
+      <c r="E131">
+        <v>62.58</v>
+      </c>
+      <c r="F131">
+        <v>61.16</v>
+      </c>
+      <c r="G131">
+        <v>60.85</v>
+      </c>
+      <c r="H131">
+        <v>60.32</v>
+      </c>
+      <c r="I131">
+        <v>58.35</v>
+      </c>
+      <c r="J131">
+        <v>59.77</v>
+      </c>
+      <c r="K131">
+        <v>59.12</v>
+      </c>
+      <c r="L131">
+        <v>59.53</v>
+      </c>
+      <c r="M131">
+        <v>53.93</v>
+      </c>
+      <c r="N131">
+        <v>49.83</v>
+      </c>
+      <c r="O131">
+        <v>46.76</v>
+      </c>
+      <c r="P131">
+        <v>44.84</v>
+      </c>
+      <c r="Q131">
+        <v>39.42</v>
+      </c>
+      <c r="R131">
+        <v>36.92</v>
+      </c>
+      <c r="S131">
+        <v>36.6</v>
+      </c>
+      <c r="T131">
+        <v>34.78</v>
+      </c>
+      <c r="U131">
+        <v>34.01</v>
+      </c>
+      <c r="V131">
+        <v>30.15</v>
+      </c>
+      <c r="W131">
+        <v>30.78</v>
+      </c>
+      <c r="X131">
+        <v>33.18</v>
+      </c>
+      <c r="Y131">
+        <v>32.159999999999997</v>
+      </c>
+    </row>
+    <row r="132" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A132" t="s">
+        <v>42</v>
+      </c>
+      <c r="B132">
+        <v>0.59</v>
+      </c>
+      <c r="C132">
+        <v>0.6</v>
+      </c>
+      <c r="D132">
+        <v>0.64</v>
+      </c>
+      <c r="E132">
+        <v>0.68</v>
+      </c>
+      <c r="F132">
+        <v>0.75</v>
+      </c>
+      <c r="G132">
+        <v>0.89</v>
+      </c>
+      <c r="H132">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I132">
+        <v>1.44</v>
+      </c>
+      <c r="J132">
+        <v>1.62</v>
+      </c>
+      <c r="K132">
+        <v>2.09</v>
+      </c>
+      <c r="L132">
+        <v>3.38</v>
+      </c>
+      <c r="M132">
+        <v>5.64</v>
+      </c>
+      <c r="N132">
+        <v>8.61</v>
+      </c>
+      <c r="O132">
+        <v>13.25</v>
+      </c>
+      <c r="P132">
+        <v>18.11</v>
+      </c>
+      <c r="Q132">
+        <v>24.24</v>
+      </c>
+      <c r="R132">
+        <v>35.43</v>
+      </c>
+      <c r="S132">
+        <v>43.77</v>
+      </c>
+      <c r="T132">
+        <v>51.99</v>
+      </c>
+      <c r="U132">
+        <v>61.59</v>
+      </c>
+      <c r="V132">
+        <v>76.44</v>
+      </c>
+      <c r="W132">
+        <v>95.39</v>
+      </c>
+      <c r="X132">
+        <v>114.36</v>
+      </c>
+      <c r="Y132">
+        <v>139.21</v>
+      </c>
+    </row>
+    <row r="133" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A133" t="s">
+        <v>43</v>
+      </c>
+      <c r="B133">
+        <v>2.38</v>
+      </c>
+      <c r="C133">
+        <v>3.86</v>
+      </c>
+      <c r="D133">
+        <v>4.42</v>
+      </c>
+      <c r="E133">
+        <v>6</v>
+      </c>
+      <c r="F133">
+        <v>6.46</v>
+      </c>
+      <c r="G133">
+        <v>8.7100000000000009</v>
+      </c>
+      <c r="H133">
+        <v>11.33</v>
+      </c>
+      <c r="I133">
+        <v>16.52</v>
+      </c>
+      <c r="J133">
+        <v>24.65</v>
+      </c>
+      <c r="K133">
+        <v>34.299999999999997</v>
+      </c>
+      <c r="L133">
+        <v>39.35</v>
+      </c>
+      <c r="M133">
+        <v>45.79</v>
+      </c>
+      <c r="N133">
+        <v>59.45</v>
+      </c>
+      <c r="O133">
+        <v>60.2</v>
+      </c>
+      <c r="P133">
+        <v>64.430000000000007</v>
+      </c>
+      <c r="Q133">
+        <v>72.77</v>
+      </c>
+      <c r="R133">
+        <v>81.5</v>
+      </c>
+      <c r="S133">
+        <v>87.83</v>
+      </c>
+      <c r="T133">
+        <v>94.67</v>
+      </c>
+      <c r="U133">
+        <v>103.84</v>
+      </c>
+      <c r="V133">
+        <v>118.66</v>
+      </c>
+      <c r="W133">
+        <v>133.02000000000001</v>
+      </c>
+      <c r="X133">
+        <v>141.66999999999999</v>
+      </c>
+      <c r="Y133">
+        <v>148.02000000000001</v>
+      </c>
+    </row>
+    <row r="139" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A139" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="140" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A140" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="141" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A141" t="s">
+        <v>38</v>
+      </c>
+      <c r="B141">
+        <v>2000</v>
+      </c>
+      <c r="C141">
+        <v>2001</v>
+      </c>
+      <c r="D141">
+        <v>2002</v>
+      </c>
+      <c r="E141">
+        <v>2003</v>
+      </c>
+      <c r="F141">
+        <v>2004</v>
+      </c>
+      <c r="G141">
+        <v>2005</v>
+      </c>
+      <c r="H141">
+        <v>2006</v>
+      </c>
+      <c r="I141">
+        <v>2007</v>
+      </c>
+      <c r="J141">
+        <v>2008</v>
+      </c>
+      <c r="K141">
+        <v>2009</v>
+      </c>
+      <c r="L141">
+        <v>2010</v>
+      </c>
+      <c r="M141">
+        <v>2011</v>
+      </c>
+      <c r="N141">
+        <v>2012</v>
+      </c>
+      <c r="O141">
+        <v>2013</v>
+      </c>
+      <c r="P141">
+        <v>2014</v>
+      </c>
+      <c r="Q141">
+        <v>2015</v>
+      </c>
+      <c r="R141">
+        <v>2016</v>
+      </c>
+      <c r="S141">
+        <v>2017</v>
+      </c>
+      <c r="T141">
+        <v>2018</v>
+      </c>
+      <c r="U141">
+        <v>2019</v>
+      </c>
+      <c r="V141">
+        <v>2020</v>
+      </c>
+      <c r="W141">
+        <v>2021</v>
+      </c>
+      <c r="X141">
+        <v>2022</v>
+      </c>
+      <c r="Y141">
+        <v>2023</v>
+      </c>
+      <c r="Z141">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="142" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A142" t="s">
+        <v>31</v>
+      </c>
+      <c r="B142">
+        <v>6.796149999999999</v>
+      </c>
+      <c r="C142">
+        <v>8.3813949999999995</v>
+      </c>
+      <c r="D142">
+        <v>8.4054149999999996</v>
+      </c>
+      <c r="E142">
+        <v>8.4073600000000006</v>
+      </c>
+      <c r="F142">
+        <v>8.6129899999999999</v>
+      </c>
+      <c r="G142">
+        <v>8.7186249999999994</v>
+      </c>
+      <c r="H142">
+        <v>9.0057599999999987</v>
+      </c>
+      <c r="I142">
+        <v>9.7297499999999992</v>
+      </c>
+      <c r="J142">
+        <v>9.9424499999999991</v>
+      </c>
+      <c r="K142">
+        <v>10.142300000000001</v>
+      </c>
+      <c r="L142">
+        <v>10.295999999999999</v>
+      </c>
+      <c r="M142">
+        <v>10.493450000000001</v>
+      </c>
+      <c r="N142">
+        <v>11.216849999999999</v>
+      </c>
+      <c r="O142">
+        <v>12.283349999999999</v>
+      </c>
+      <c r="P142">
+        <v>12.419550000000001</v>
+      </c>
+      <c r="Q142">
+        <v>12.9693</v>
+      </c>
+      <c r="R142">
+        <v>12.900699999999999</v>
+      </c>
+      <c r="S142">
+        <v>12.837900000000001</v>
+      </c>
+      <c r="T142">
+        <v>12.616149999999999</v>
+      </c>
+      <c r="U142">
+        <v>12.052950000000001</v>
+      </c>
+      <c r="V142">
+        <v>11.8889</v>
+      </c>
+      <c r="W142">
+        <v>11.334</v>
+      </c>
+      <c r="X142">
+        <v>11.1015</v>
+      </c>
+      <c r="Y142">
+        <v>10.9895</v>
+      </c>
+      <c r="Z142">
+        <v>10.9101</v>
+      </c>
+    </row>
+    <row r="143" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A143" t="s">
+        <v>33</v>
+      </c>
+      <c r="B143">
+        <v>321.05500000000001</v>
+      </c>
+      <c r="C143">
+        <v>315.09773999999999</v>
+      </c>
+      <c r="D143">
+        <v>316.19997999999998</v>
+      </c>
+      <c r="E143">
+        <v>313.87878000000001</v>
+      </c>
+      <c r="F143">
+        <v>314.02522999999997</v>
+      </c>
+      <c r="G143">
+        <v>314.28313000000003</v>
+      </c>
+      <c r="H143">
+        <v>313.87216999999998</v>
+      </c>
+      <c r="I143">
+        <v>313.64070000000004</v>
+      </c>
+      <c r="J143">
+        <v>314.23070000000001</v>
+      </c>
+      <c r="K143">
+        <v>315.13</v>
+      </c>
+      <c r="L143">
+        <v>317.73700000000002</v>
+      </c>
+      <c r="M143">
+        <v>318.58100000000002</v>
+      </c>
+      <c r="N143">
+        <v>310.49809999999997</v>
+      </c>
+      <c r="O143">
+        <v>304.12809999999996</v>
+      </c>
+      <c r="P143">
+        <v>299.90940000000001</v>
+      </c>
+      <c r="Q143">
+        <v>280.77350000000001</v>
+      </c>
+      <c r="R143">
+        <v>267.61500000000001</v>
+      </c>
+      <c r="S143">
+        <v>257.47339999999997</v>
+      </c>
+      <c r="T143">
+        <v>243.71170000000001</v>
+      </c>
+      <c r="U143">
+        <v>229.57550000000001</v>
+      </c>
+      <c r="V143">
+        <v>216.47229999999999</v>
+      </c>
+      <c r="W143">
+        <v>210.60479999999998</v>
+      </c>
+      <c r="X143">
+        <v>190.0273</v>
+      </c>
+      <c r="Y143">
+        <v>181.46689999999998</v>
+      </c>
+      <c r="Z143">
+        <v>177.0069</v>
+      </c>
+    </row>
+    <row r="144" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A144" t="s">
+        <v>35</v>
+      </c>
+      <c r="B144">
+        <v>243.24100000000001</v>
+      </c>
+      <c r="C144">
+        <v>233.81331</v>
+      </c>
+      <c r="D144">
+        <v>313.74014</v>
+      </c>
+      <c r="E144">
+        <v>356.62590999999998</v>
+      </c>
+      <c r="F144">
+        <v>372.10201000000001</v>
+      </c>
+      <c r="G144">
+        <v>383.88529</v>
+      </c>
+      <c r="H144">
+        <v>389.38721000000004</v>
+      </c>
+      <c r="I144">
+        <v>393.9015</v>
+      </c>
+      <c r="J144">
+        <v>398.26979999999998</v>
+      </c>
+      <c r="K144">
+        <v>402.02679999999998</v>
+      </c>
+      <c r="L144">
+        <v>406.87579999999997</v>
+      </c>
+      <c r="M144">
+        <v>416.1848</v>
+      </c>
+      <c r="N144">
+        <v>423.4923</v>
+      </c>
+      <c r="O144">
+        <v>426.67570000000001</v>
+      </c>
+      <c r="P144">
+        <v>433.24940000000004</v>
+      </c>
+      <c r="Q144">
+        <v>440.87220000000002</v>
+      </c>
+      <c r="R144">
+        <v>448.28500000000003</v>
+      </c>
+      <c r="S144">
+        <v>457.46129999999999</v>
+      </c>
+      <c r="T144">
+        <v>471.85470000000004</v>
+      </c>
+      <c r="U144">
+        <v>478.14850000000001</v>
+      </c>
+      <c r="V144">
+        <v>487.16429999999997</v>
+      </c>
+      <c r="W144">
+        <v>492.97909999999996</v>
+      </c>
+      <c r="X144">
+        <v>503.41409999999996</v>
+      </c>
+      <c r="Y144">
+        <v>508.3458</v>
+      </c>
+      <c r="Z144">
+        <v>506.93170000000003</v>
+      </c>
+    </row>
+    <row r="145" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A145" t="s">
+        <v>39</v>
+      </c>
+      <c r="B145">
+        <v>2.7930000000000001</v>
+      </c>
+      <c r="C145">
+        <v>2.2162100000000002</v>
+      </c>
+      <c r="D145">
+        <v>2.2522500000000001</v>
+      </c>
+      <c r="E145">
+        <v>2.1332499999999999</v>
+      </c>
+      <c r="F145">
+        <v>2.1520799999999998</v>
+      </c>
+      <c r="G145">
+        <v>2.2853000000000003</v>
+      </c>
+      <c r="H145">
+        <v>2.2739799999999999</v>
+      </c>
+      <c r="I145">
+        <v>2.2141999999999999</v>
+      </c>
+      <c r="J145">
+        <v>2.2288000000000001</v>
+      </c>
+      <c r="K145">
+        <v>2.3818999999999999</v>
+      </c>
+      <c r="L145">
+        <v>2.4045999999999998</v>
+      </c>
+      <c r="M145">
+        <v>2.4091999999999998</v>
+      </c>
+      <c r="N145">
+        <v>2.5920999999999998</v>
+      </c>
+      <c r="O145">
+        <v>2.6070000000000002</v>
+      </c>
+      <c r="P145">
+        <v>2.5143</v>
+      </c>
+      <c r="Q145">
+        <v>2.5415000000000001</v>
+      </c>
+      <c r="R145">
+        <v>2.5165999999999999</v>
+      </c>
+      <c r="S145">
+        <v>2.4833000000000003</v>
+      </c>
+      <c r="T145">
+        <v>2.4443000000000001</v>
+      </c>
+      <c r="U145">
+        <v>2.5554000000000001</v>
+      </c>
+      <c r="V145">
+        <v>2.5719000000000003</v>
+      </c>
+      <c r="W145">
+        <v>2.5966999999999998</v>
+      </c>
+      <c r="X145">
+        <v>2.6486000000000001</v>
+      </c>
+      <c r="Y145">
+        <v>2.6736</v>
+      </c>
+      <c r="Z145">
+        <v>2.7028000000000003</v>
+      </c>
+    </row>
+    <row r="146" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A146" t="s">
+        <v>40</v>
+      </c>
+      <c r="B146">
+        <v>97.600000000000009</v>
+      </c>
+      <c r="C146">
+        <v>98.580000000000013</v>
+      </c>
+      <c r="D146">
+        <v>99.727000000000004</v>
+      </c>
+      <c r="E146">
+        <v>99.215999999999994</v>
+      </c>
+      <c r="F146">
+        <v>98.405000000000001</v>
+      </c>
+      <c r="G146">
+        <v>98.887</v>
+      </c>
+      <c r="H146">
+        <v>99.282000000000011</v>
+      </c>
+      <c r="I146">
+        <v>99.770999999999987</v>
+      </c>
+      <c r="J146">
+        <v>99.787999999999997</v>
+      </c>
+      <c r="K146">
+        <v>100.678</v>
+      </c>
+      <c r="L146">
+        <v>101.1204</v>
+      </c>
+      <c r="M146">
+        <v>101.0419</v>
+      </c>
+      <c r="N146">
+        <v>101.2259</v>
+      </c>
+      <c r="O146">
+        <v>101.69289999999999</v>
+      </c>
+      <c r="P146">
+        <v>102.27019999999999</v>
+      </c>
+      <c r="Q146">
+        <v>102.36019999999999</v>
+      </c>
+      <c r="R146">
+        <v>102.84774899999999</v>
+      </c>
+      <c r="S146">
+        <v>102.85131799999999</v>
+      </c>
+      <c r="T146">
+        <v>102.960565</v>
+      </c>
+      <c r="U146">
+        <v>102.814713</v>
+      </c>
+      <c r="V146">
+        <v>103.188447</v>
+      </c>
+      <c r="W146">
+        <v>103.159282</v>
+      </c>
+      <c r="X146">
+        <v>103.33971200000001</v>
+      </c>
+      <c r="Y146">
+        <v>103.25035299999999</v>
+      </c>
+      <c r="Z146">
+        <v>103.103253</v>
+      </c>
+    </row>
+    <row r="147" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A147" t="s">
+        <v>41</v>
+      </c>
+      <c r="B147">
+        <v>97.86</v>
+      </c>
+      <c r="C147">
+        <v>98.158899999999988</v>
+      </c>
+      <c r="D147">
+        <v>98.656999999999996</v>
+      </c>
+      <c r="E147">
+        <v>99.208860000000001</v>
+      </c>
+      <c r="F147">
+        <v>99.628100000000003</v>
+      </c>
+      <c r="G147">
+        <v>99.988039999999998</v>
+      </c>
+      <c r="H147">
+        <v>100.33377</v>
+      </c>
+      <c r="I147">
+        <v>100.2657</v>
+      </c>
+      <c r="J147">
+        <v>100.75489999999999</v>
+      </c>
+      <c r="K147">
+        <v>101.00369999999999</v>
+      </c>
+      <c r="L147">
+        <v>101.1674</v>
+      </c>
+      <c r="M147">
+        <v>101.4188</v>
+      </c>
+      <c r="N147">
+        <v>101.88500000000001</v>
+      </c>
+      <c r="O147">
+        <v>99.240300000000005</v>
+      </c>
+      <c r="P147">
+        <v>98.569299999999998</v>
+      </c>
+      <c r="Q147">
+        <v>98.671999999999997</v>
+      </c>
+      <c r="R147">
+        <v>99.564800000000005</v>
+      </c>
+      <c r="S147">
+        <v>99.628899999999987</v>
+      </c>
+      <c r="T147">
+        <v>99.432899999999989</v>
+      </c>
+      <c r="U147">
+        <v>98.119</v>
+      </c>
+      <c r="V147">
+        <v>96.500600000000006</v>
+      </c>
+      <c r="W147">
+        <v>95.546399999999991</v>
+      </c>
+      <c r="X147">
+        <v>94.658899999999988</v>
+      </c>
+      <c r="Y147">
+        <v>95.772899999999993</v>
+      </c>
+      <c r="Z147">
+        <v>96.886899999999997</v>
+      </c>
+    </row>
+    <row r="148" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A148" t="s">
+        <v>37</v>
+      </c>
+      <c r="B148">
+        <v>86.087164999999999</v>
+      </c>
+      <c r="C148">
+        <v>87.751305000000002</v>
+      </c>
+      <c r="D148">
+        <v>61.516044999999998</v>
+      </c>
+      <c r="E148">
+        <v>62.584490000000002</v>
+      </c>
+      <c r="F148">
+        <v>61.162999999999997</v>
+      </c>
+      <c r="G148">
+        <v>60.854835000000001</v>
+      </c>
+      <c r="H148">
+        <v>60.320080000000004</v>
+      </c>
+      <c r="I148">
+        <v>58.348350000000003</v>
+      </c>
+      <c r="J148">
+        <v>59.769349999999996</v>
+      </c>
+      <c r="K148">
+        <v>59.1233</v>
+      </c>
+      <c r="L148">
+        <v>59.525500000000001</v>
+      </c>
+      <c r="M148">
+        <v>53.92915</v>
+      </c>
+      <c r="N148">
+        <v>49.832649999999994</v>
+      </c>
+      <c r="O148">
+        <v>46.755250000000004</v>
+      </c>
+      <c r="P148">
+        <v>44.843950000000007</v>
+      </c>
+      <c r="Q148">
+        <v>39.415800000000004</v>
+      </c>
+      <c r="R148">
+        <v>36.920600000000007</v>
+      </c>
+      <c r="S148">
+        <v>36.6036</v>
+      </c>
+      <c r="T148">
+        <v>34.782850000000003</v>
+      </c>
+      <c r="U148">
+        <v>34.005249999999997</v>
+      </c>
+      <c r="V148">
+        <v>30.154299999999999</v>
+      </c>
+      <c r="W148">
+        <v>30.7805</v>
+      </c>
+      <c r="X148">
+        <v>33.178799999999995</v>
+      </c>
+      <c r="Y148">
+        <v>32.158799999999999</v>
+      </c>
+      <c r="Z148">
+        <v>31.953700000000001</v>
+      </c>
+    </row>
+    <row r="149" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A149" t="s">
+        <v>42</v>
+      </c>
+      <c r="B149">
+        <v>0.59371299999999994</v>
+      </c>
+      <c r="C149">
+        <v>0.59860000000000002</v>
+      </c>
+      <c r="D149">
+        <v>0.64260000000000006</v>
+      </c>
+      <c r="E149">
+        <v>0.68100000000000005</v>
+      </c>
+      <c r="F149">
+        <v>0.75180000000000002</v>
+      </c>
+      <c r="G149">
+        <v>0.89379999999999993</v>
+      </c>
+      <c r="H149">
+        <v>1.0988</v>
+      </c>
+      <c r="I149">
+        <v>1.4388000000000001</v>
+      </c>
+      <c r="J149">
+        <v>1.6177999999999999</v>
+      </c>
+      <c r="K149">
+        <v>2.0870000000000002</v>
+      </c>
+      <c r="L149">
+        <v>3.3819999999999997</v>
+      </c>
+      <c r="M149">
+        <v>5.6434999999999995</v>
+      </c>
+      <c r="N149">
+        <v>8.6129999999999995</v>
+      </c>
+      <c r="O149">
+        <v>13.245500000000002</v>
+      </c>
+      <c r="P149">
+        <v>18.112127999999998</v>
+      </c>
+      <c r="Q149">
+        <v>24.236846</v>
+      </c>
+      <c r="R149">
+        <v>35.433673999999996</v>
+      </c>
+      <c r="S149">
+        <v>43.769840000000002</v>
+      </c>
+      <c r="T149">
+        <v>51.986993999999996</v>
+      </c>
+      <c r="U149">
+        <v>61.587229000000001</v>
+      </c>
+      <c r="V149">
+        <v>76.441096999999999</v>
+      </c>
+      <c r="W149">
+        <v>95.390912999999998</v>
+      </c>
+      <c r="X149">
+        <v>114.36094700000001</v>
+      </c>
+      <c r="Y149">
+        <v>139.205277</v>
+      </c>
+      <c r="Z149">
+        <v>177.47027699999998</v>
+      </c>
+    </row>
+    <row r="150" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A150" t="s">
+        <v>43</v>
+      </c>
+      <c r="B150">
+        <v>2.3769999999999998</v>
+      </c>
+      <c r="C150">
+        <v>3.8636399999999997</v>
+      </c>
+      <c r="D150">
+        <v>4.4166400000000001</v>
+      </c>
+      <c r="E150">
+        <v>5.99519</v>
+      </c>
+      <c r="F150">
+        <v>6.4558</v>
+      </c>
+      <c r="G150">
+        <v>8.70641</v>
+      </c>
+      <c r="H150">
+        <v>11.328790000000001</v>
+      </c>
+      <c r="I150">
+        <v>16.515099999999997</v>
+      </c>
+      <c r="J150">
+        <v>24.651299999999999</v>
+      </c>
+      <c r="K150">
+        <v>34.2958</v>
+      </c>
+      <c r="L150">
+        <v>39.349694999999997</v>
+      </c>
+      <c r="M150">
+        <v>45.794967999999997</v>
+      </c>
+      <c r="N150">
+        <v>59.453299000000001</v>
+      </c>
+      <c r="O150">
+        <v>60.198163999999998</v>
+      </c>
+      <c r="P150">
+        <v>64.430186000000006</v>
+      </c>
+      <c r="Q150">
+        <v>72.767236000000011</v>
+      </c>
+      <c r="R150">
+        <v>81.502362000000005</v>
+      </c>
+      <c r="S150">
+        <v>87.830780000000004</v>
+      </c>
+      <c r="T150">
+        <v>94.666184999999999</v>
+      </c>
+      <c r="U150">
+        <v>103.835556</v>
+      </c>
+      <c r="V150">
+        <v>118.66354000000001</v>
+      </c>
+      <c r="W150">
+        <v>133.01927700000002</v>
+      </c>
+      <c r="X150">
+        <v>141.673912</v>
+      </c>
+      <c r="Y150">
+        <v>148.01986099999999</v>
+      </c>
+      <c r="Z150">
+        <v>153.15226100000001</v>
+      </c>
+    </row>
+    <row r="156" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A156" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="157" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A157" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="158" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A158" t="s">
+        <v>38</v>
+      </c>
+      <c r="B158">
+        <v>2000</v>
+      </c>
+      <c r="C158">
+        <v>2001</v>
+      </c>
+      <c r="D158">
+        <v>2002</v>
+      </c>
+      <c r="E158">
+        <v>2003</v>
+      </c>
+      <c r="F158">
+        <v>2004</v>
+      </c>
+      <c r="G158">
+        <v>2005</v>
+      </c>
+      <c r="H158">
+        <v>2006</v>
+      </c>
+      <c r="I158">
+        <v>2007</v>
+      </c>
+      <c r="J158">
+        <v>2008</v>
+      </c>
+      <c r="K158">
+        <v>2009</v>
+      </c>
+      <c r="L158">
+        <v>2010</v>
+      </c>
+      <c r="M158">
+        <v>2011</v>
+      </c>
+      <c r="N158">
+        <v>2012</v>
+      </c>
+      <c r="O158">
+        <v>2013</v>
+      </c>
+      <c r="P158">
+        <v>2014</v>
+      </c>
+      <c r="Q158">
+        <v>2015</v>
+      </c>
+      <c r="R158">
+        <v>2016</v>
+      </c>
+      <c r="S158">
+        <v>2017</v>
+      </c>
+      <c r="T158">
+        <v>2018</v>
+      </c>
+      <c r="U158">
+        <v>2019</v>
+      </c>
+      <c r="V158">
+        <v>2020</v>
+      </c>
+      <c r="W158">
+        <v>2021</v>
+      </c>
+      <c r="X158">
+        <v>2022</v>
+      </c>
+      <c r="Y158">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="159" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A159" t="s">
+        <v>31</v>
+      </c>
+      <c r="B159">
+        <v>0.89062522319196646</v>
+      </c>
+      <c r="C159">
+        <v>0.69678899280358397</v>
+      </c>
+      <c r="D159">
+        <v>0.74800603116673936</v>
+      </c>
+      <c r="E159">
+        <v>0.76020465632121148</v>
+      </c>
+      <c r="F159">
+        <v>0.74784420566617438</v>
+      </c>
+      <c r="G159">
+        <v>0.73599003735990043</v>
+      </c>
+      <c r="H159">
+        <v>0.72227484698338673</v>
+      </c>
+      <c r="I159">
+        <v>0.69066795163029759</v>
+      </c>
+      <c r="J159">
+        <v>0.67864687100175214</v>
+      </c>
+      <c r="K159">
+        <v>0.65559552052243575</v>
+      </c>
+      <c r="L159">
+        <v>0.66443749325854817</v>
+      </c>
+      <c r="M159">
+        <v>0.66201196417825925</v>
+      </c>
+      <c r="N159">
+        <v>0.62723392155112279</v>
+      </c>
+      <c r="O159">
+        <v>0.61041243088585706</v>
+      </c>
+      <c r="P159">
+        <v>0.63515584141518866</v>
+      </c>
+      <c r="Q159">
+        <v>0.60865638092548136</v>
+      </c>
+      <c r="R159">
+        <v>0.60645902551984321</v>
+      </c>
+      <c r="S159">
+        <v>0.60890247135321263</v>
+      </c>
+      <c r="T159">
+        <v>0.6103440120795357</v>
+      </c>
+      <c r="U159">
+        <v>0.58898171328201421</v>
+      </c>
+      <c r="V159">
+        <v>0.57464458717798117</v>
+      </c>
+      <c r="W159">
+        <v>0.59362368402088539</v>
+      </c>
+      <c r="X159">
+        <v>0.5812370278123703</v>
+      </c>
+      <c r="Y159">
+        <v>0.54863047126229303</v>
+      </c>
+    </row>
+    <row r="160" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A160" t="s">
+        <v>33</v>
+      </c>
+      <c r="B160">
+        <v>0.67155351143519759</v>
+      </c>
+      <c r="C160">
+        <v>0.64817795527696032</v>
+      </c>
+      <c r="D160">
+        <v>0.65716778034326806</v>
+      </c>
+      <c r="E160">
+        <v>0.67364123953756039</v>
+      </c>
+      <c r="F160">
+        <v>0.67517738977915964</v>
+      </c>
+      <c r="G160">
+        <v>0.68666790295340163</v>
+      </c>
+      <c r="H160">
+        <v>0.67841156311510031</v>
+      </c>
+      <c r="I160">
+        <v>0.68993375409691593</v>
+      </c>
+      <c r="J160">
+        <v>0.67757501708780188</v>
+      </c>
+      <c r="K160">
+        <v>0.59666965969950614</v>
+      </c>
+      <c r="L160">
+        <v>0.62139867362470103</v>
+      </c>
+      <c r="M160">
+        <v>0.58165825098854018</v>
+      </c>
+      <c r="N160">
+        <v>0.5192129789664629</v>
+      </c>
+      <c r="O160">
+        <v>0.55046512285345728</v>
+      </c>
+      <c r="P160">
+        <v>0.55835395597472026</v>
+      </c>
+      <c r="Q160">
+        <v>0.51169520945224101</v>
+      </c>
+      <c r="R160">
+        <v>0.49503229904481122</v>
+      </c>
+      <c r="S160">
+        <v>0.49715749796492947</v>
+      </c>
+      <c r="T160">
+        <v>0.50285617794482929</v>
+      </c>
+      <c r="U160">
+        <v>0.45016449179220486</v>
+      </c>
+      <c r="V160">
+        <v>0.37884710642106634</v>
+      </c>
+      <c r="W160">
+        <v>0.45643802273081685</v>
+      </c>
+      <c r="X160">
+        <v>0.45213505228499729</v>
+      </c>
+      <c r="Y160">
+        <v>0.38479804073384022</v>
+      </c>
+    </row>
+    <row r="161" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A161" t="s">
+        <v>35</v>
+      </c>
+      <c r="B161">
+        <v>0.43459414324342821</v>
+      </c>
+      <c r="C161">
+        <v>0.36540314349727282</v>
+      </c>
+      <c r="D161">
+        <v>0.29817584612105158</v>
+      </c>
+      <c r="E161">
+        <v>0.23254337785044626</v>
+      </c>
+      <c r="F161">
+        <v>0.2357265436652799</v>
+      </c>
+      <c r="G161">
+        <v>0.24140612469062864</v>
+      </c>
+      <c r="H161">
+        <v>0.2511274034489509</v>
+      </c>
+      <c r="I161">
+        <v>0.27007535324960963</v>
+      </c>
+      <c r="J161">
+        <v>0.25948462775896008</v>
+      </c>
+      <c r="K161">
+        <v>0.26346248138415496</v>
+      </c>
+      <c r="L161">
+        <v>0.27698219360923532</v>
+      </c>
+      <c r="M161">
+        <v>0.27663886332699111</v>
+      </c>
+      <c r="N161">
+        <v>0.32619701364051612</v>
+      </c>
+      <c r="O161">
+        <v>0.29366142042277804</v>
+      </c>
+      <c r="P161">
+        <v>0.28649687567071613</v>
+      </c>
+      <c r="Q161">
+        <v>0.33065522143544857</v>
+      </c>
+      <c r="R161">
+        <v>0.33263847318431589</v>
+      </c>
+      <c r="S161">
+        <v>0.30521444820465338</v>
+      </c>
+      <c r="T161">
+        <v>0.32944173514367192</v>
+      </c>
+      <c r="U161">
+        <v>0.3486145024125431</v>
+      </c>
+      <c r="V161">
+        <v>0.35400006538725604</v>
+      </c>
+      <c r="W161">
+        <v>0.33997063902656871</v>
+      </c>
+      <c r="X161">
+        <v>0.3596458533135401</v>
+      </c>
+      <c r="Y161">
+        <v>0.37973814833719327</v>
+      </c>
+    </row>
+    <row r="162" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A162" t="s">
+        <v>40</v>
+      </c>
+      <c r="B162">
+        <v>0.38842417421564296</v>
+      </c>
+      <c r="C162">
+        <v>0.30106784050434288</v>
+      </c>
+      <c r="D162">
+        <v>0.36765298184563266</v>
+      </c>
+      <c r="E162">
+        <v>0.3877274618452502</v>
+      </c>
+      <c r="F162">
+        <v>0.3821789596757309</v>
+      </c>
+      <c r="G162">
+        <v>0.38831040806159256</v>
+      </c>
+      <c r="H162">
+        <v>0.41468193196100595</v>
+      </c>
+      <c r="I162">
+        <v>0.35268226729800917</v>
+      </c>
+      <c r="J162">
+        <v>0.36407219451714945</v>
+      </c>
+      <c r="K162">
+        <v>0.39082035929536607</v>
+      </c>
+      <c r="L162">
+        <v>0.35195911470467772</v>
+      </c>
+      <c r="M162">
+        <v>0.43326382946908459</v>
+      </c>
+      <c r="N162">
+        <v>0.37511116863119892</v>
+      </c>
+      <c r="O162">
+        <v>0.36288745538167544</v>
+      </c>
+      <c r="P162">
+        <v>0.34618478903497041</v>
+      </c>
+      <c r="Q162">
+        <v>0.33356574522188498</v>
+      </c>
+      <c r="R162">
+        <v>0.355635417926433</v>
+      </c>
+      <c r="S162">
+        <v>0.40032675731511858</v>
+      </c>
+      <c r="T162">
+        <v>0.39007126945865267</v>
+      </c>
+      <c r="U162">
+        <v>0.3850270381324043</v>
+      </c>
+      <c r="V162">
+        <v>0.38122107308931918</v>
+      </c>
+      <c r="W162">
+        <v>0.33379813440335088</v>
+      </c>
+      <c r="X162">
+        <v>0.32779937982191626</v>
+      </c>
+      <c r="Y162">
+        <v>0.31484244836536429</v>
+      </c>
+    </row>
+    <row r="163" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A163" t="s">
+        <v>41</v>
+      </c>
+      <c r="B163">
+        <v>0.87942471166058678</v>
+      </c>
+      <c r="C163">
+        <v>0.89411146836959887</v>
+      </c>
+      <c r="D163">
+        <v>0.90257394288951398</v>
+      </c>
+      <c r="E163">
+        <v>0.87878026362602468</v>
+      </c>
+      <c r="F163">
+        <v>0.90349131970940888</v>
+      </c>
+      <c r="G163">
+        <v>0.89277192559438601</v>
+      </c>
+      <c r="H163">
+        <v>0.89569716738416194</v>
+      </c>
+      <c r="I163">
+        <v>0.91809192804997286</v>
+      </c>
+      <c r="J163">
+        <v>0.91347995059881948</v>
+      </c>
+      <c r="K163">
+        <v>0.90290022152900229</v>
+      </c>
+      <c r="L163">
+        <v>0.91054525070375247</v>
+      </c>
+      <c r="M163">
+        <v>0.8894249600873082</v>
+      </c>
+      <c r="N163">
+        <v>0.86193992895014826</v>
+      </c>
+      <c r="O163">
+        <v>0.90760556484993726</v>
+      </c>
+      <c r="P163">
+        <v>0.92321336666847342</v>
+      </c>
+      <c r="Q163">
+        <v>0.92228927845366193</v>
+      </c>
+      <c r="R163">
+        <v>0.92380217248129226</v>
+      </c>
+      <c r="S163">
+        <v>0.92230522339047183</v>
+      </c>
+      <c r="T163">
+        <v>0.92660585428265319</v>
+      </c>
+      <c r="U163">
+        <v>0.94168774792584609</v>
+      </c>
+      <c r="V163">
+        <v>0.9343932618827927</v>
+      </c>
+      <c r="W163">
+        <v>0.93146145005244818</v>
+      </c>
+      <c r="X163">
+        <v>0.93043885976921004</v>
+      </c>
+      <c r="Y163">
+        <v>0.92362409368335385</v>
+      </c>
+    </row>
+    <row r="164" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A164" t="s">
+        <v>37</v>
+      </c>
+      <c r="B164">
+        <v>0.15384240024907564</v>
+      </c>
+      <c r="C164">
+        <v>0.17639100287502116</v>
+      </c>
+      <c r="D164">
+        <v>0.19240503886325713</v>
+      </c>
+      <c r="E164">
+        <v>0.24148085883858617</v>
+      </c>
+      <c r="F164">
+        <v>0.24242125602133488</v>
+      </c>
+      <c r="G164">
+        <v>0.23662122968749411</v>
+      </c>
+      <c r="H164">
+        <v>0.13552151084626285</v>
+      </c>
+      <c r="I164">
+        <v>0.14710082833476149</v>
+      </c>
+      <c r="J164">
+        <v>0.10586624679230811</v>
+      </c>
+      <c r="K164">
+        <v>9.370694076284751E-2</v>
+      </c>
+      <c r="L164">
+        <v>9.1086417423546853E-2</v>
+      </c>
+      <c r="M164">
+        <v>8.8500483037795494E-2</v>
+      </c>
+      <c r="N164">
+        <v>8.9551048908755537E-2</v>
+      </c>
+      <c r="O164">
+        <v>9.8286792364390599E-2</v>
+      </c>
+      <c r="P164">
+        <v>0.1112275406417134</v>
+      </c>
+      <c r="Q164">
+        <v>0.12869252564004549</v>
+      </c>
+      <c r="R164">
+        <v>0.12213251408698061</v>
+      </c>
+      <c r="S164">
+        <v>0.11817875589490232</v>
+      </c>
+      <c r="T164">
+        <v>0.140084707266287</v>
+      </c>
+      <c r="U164">
+        <v>0.12566811534077407</v>
+      </c>
+      <c r="V164">
+        <v>0.13001961274298221</v>
+      </c>
+      <c r="W164">
+        <v>0.13054791553549863</v>
+      </c>
+      <c r="X164">
+        <v>0.13294029246864345</v>
+      </c>
+      <c r="Y164">
+        <v>0.11759836661441653</v>
+      </c>
+    </row>
+    <row r="165" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A165" t="s">
+        <v>42</v>
+      </c>
+      <c r="B165">
+        <v>9.4806903490441935E-2</v>
+      </c>
+      <c r="C165">
+        <v>0.10273972602739728</v>
+      </c>
+      <c r="D165">
+        <v>9.8102168949771695E-2</v>
+      </c>
+      <c r="E165">
+        <v>8.8973945742680638E-2</v>
+      </c>
+      <c r="F165">
+        <v>8.8280060882800604E-2</v>
+      </c>
+      <c r="G165">
+        <v>7.0545379918936946E-2</v>
+      </c>
+      <c r="H165">
+        <v>5.2926525529265252E-2</v>
+      </c>
+      <c r="I165">
+        <v>4.8357432775240995E-2</v>
+      </c>
+      <c r="J165">
+        <v>6.0600935791194542E-2</v>
+      </c>
+      <c r="K165">
+        <v>4.8611566275589352E-2</v>
+      </c>
+      <c r="L165">
+        <v>4.0866228958958146E-2</v>
+      </c>
+      <c r="M165">
+        <v>3.6837332815181839E-2</v>
+      </c>
+      <c r="N165">
+        <v>5.7409086811024669E-2</v>
+      </c>
+      <c r="O165">
+        <v>7.7884035495821485E-2</v>
+      </c>
+      <c r="P165">
+        <v>0.18229540933261729</v>
+      </c>
+      <c r="Q165">
+        <v>0.18380690808806913</v>
+      </c>
+      <c r="R165">
+        <v>0.17679081654352205</v>
+      </c>
+      <c r="S165">
+        <v>0.20155169769749093</v>
+      </c>
+      <c r="T165">
+        <v>0.20499200320398811</v>
+      </c>
+      <c r="U165">
+        <v>0.19811746703231933</v>
+      </c>
+      <c r="V165">
+        <v>0.19521682926770992</v>
+      </c>
+      <c r="W165">
+        <v>0.19676492706461959</v>
+      </c>
+      <c r="X165">
+        <v>0.2047028449772488</v>
+      </c>
+      <c r="Y165">
+        <v>0.19593603697839634</v>
+      </c>
+    </row>
+    <row r="166" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A166" t="s">
+        <v>43</v>
+      </c>
+      <c r="B166">
+        <v>0.26812094700894057</v>
+      </c>
+      <c r="C166">
+        <v>0.19932808100882485</v>
+      </c>
+      <c r="D166">
+        <v>0.26730924192648609</v>
+      </c>
+      <c r="E166">
+        <v>0.21289954337899542</v>
+      </c>
+      <c r="F166">
+        <v>0.24986923392284097</v>
+      </c>
+      <c r="G166">
+        <v>0.23342193143869688</v>
+      </c>
+      <c r="H166">
+        <v>0.26790716044606189</v>
+      </c>
+      <c r="I166">
+        <v>0.23805377735027147</v>
+      </c>
+      <c r="J166">
+        <v>0.25637463298970986</v>
+      </c>
+      <c r="K166">
+        <v>0.2459163704620792</v>
+      </c>
+      <c r="L166">
+        <v>0.27458181754886773</v>
+      </c>
+      <c r="M166">
+        <v>0.29961079017671505</v>
+      </c>
+      <c r="N166">
+        <v>0.27040105072755966</v>
+      </c>
+      <c r="O166">
+        <v>0.31826939122256104</v>
+      </c>
+      <c r="P166">
+        <v>0.32184233074442048</v>
+      </c>
+      <c r="Q166">
+        <v>0.29918495942994222</v>
+      </c>
+      <c r="R166">
+        <v>0.31793988290332525</v>
+      </c>
+      <c r="S166">
+        <v>0.33052123836157127</v>
+      </c>
+      <c r="T166">
+        <v>0.32879172207422758</v>
+      </c>
+      <c r="U166">
+        <v>0.32527210812560242</v>
+      </c>
+      <c r="V166">
+        <v>0.32511061495681998</v>
+      </c>
+      <c r="W166">
+        <v>0.32456409548740911</v>
+      </c>
+      <c r="X166">
+        <v>0.34995147575899105</v>
+      </c>
+      <c r="Y166">
+        <v>0.32478950456528455</v>
+      </c>
+    </row>
+    <row r="174" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A174" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="175" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A175" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="176" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A176" t="s">
+        <v>38</v>
+      </c>
+      <c r="B176">
+        <v>2000</v>
+      </c>
+      <c r="C176">
+        <v>2001</v>
+      </c>
+      <c r="D176">
+        <v>2002</v>
+      </c>
+      <c r="E176">
+        <v>2003</v>
+      </c>
+      <c r="F176">
+        <v>2004</v>
+      </c>
+      <c r="G176">
+        <v>2005</v>
+      </c>
+      <c r="H176">
+        <v>2006</v>
+      </c>
+      <c r="I176">
+        <v>2007</v>
+      </c>
+      <c r="J176">
+        <v>2008</v>
+      </c>
+      <c r="K176">
+        <v>2009</v>
+      </c>
+      <c r="L176">
+        <v>2010</v>
+      </c>
+      <c r="M176">
+        <v>2011</v>
+      </c>
+      <c r="N176">
+        <v>2012</v>
+      </c>
+      <c r="O176">
+        <v>2013</v>
+      </c>
+      <c r="P176">
+        <v>2014</v>
+      </c>
+      <c r="Q176">
+        <v>2015</v>
+      </c>
+      <c r="R176">
+        <v>2016</v>
+      </c>
+      <c r="S176">
+        <v>2017</v>
+      </c>
+      <c r="T176">
+        <v>2018</v>
+      </c>
+      <c r="U176">
+        <v>2019</v>
+      </c>
+      <c r="V176">
+        <v>2020</v>
+      </c>
+      <c r="W176">
+        <v>2021</v>
+      </c>
+      <c r="X176">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="177" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A177" t="s">
+        <v>31</v>
+      </c>
+      <c r="B177">
+        <v>0.94365811868302962</v>
+      </c>
+      <c r="C177">
+        <v>0.68559383760782999</v>
+      </c>
+      <c r="D177">
+        <v>0.73369475559619457</v>
+      </c>
+      <c r="E177">
+        <v>0.7348556644085017</v>
+      </c>
+      <c r="F177">
+        <v>0.73933935701591147</v>
+      </c>
+      <c r="G177">
+        <v>0.75916046258760472</v>
+      </c>
+      <c r="H177">
+        <v>0.74528658837440942</v>
+      </c>
+      <c r="I177">
+        <v>0.69364293783799436</v>
+      </c>
+      <c r="J177">
+        <v>0.68484310999757936</v>
+      </c>
+      <c r="K177">
+        <v>0.667656755780765</v>
+      </c>
+      <c r="L177">
+        <v>0.68457670088663258</v>
+      </c>
+      <c r="M177">
+        <v>0.67796151419614648</v>
+      </c>
+      <c r="N177">
+        <v>0.65244510546887402</v>
+      </c>
+      <c r="O177">
+        <v>0.62209726746527905</v>
+      </c>
+      <c r="P177">
+        <v>0.65092912413517146</v>
+      </c>
+      <c r="Q177">
+        <v>0.61672685798535054</v>
+      </c>
+      <c r="R177">
+        <v>0.61071513481640749</v>
+      </c>
+      <c r="S177">
+        <v>0.61227993554046112</v>
+      </c>
+      <c r="T177">
+        <v>0.61424675703319098</v>
+      </c>
+      <c r="U177">
+        <v>0.59851960113366587</v>
+      </c>
+      <c r="V177">
+        <v>0.57869297792104235</v>
+      </c>
+      <c r="W177">
+        <v>0.6001057351179182</v>
+      </c>
+      <c r="X177">
+        <v>0.58762473375085889</v>
+      </c>
+    </row>
+    <row r="178" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A178" t="s">
+        <v>33</v>
+      </c>
+      <c r="B178">
+        <v>0.75717051282625658</v>
+      </c>
+      <c r="C178">
+        <v>0.7180927619242653</v>
+      </c>
+      <c r="D178">
+        <v>0.73636459534132392</v>
+      </c>
+      <c r="E178">
+        <v>0.75768933070189082</v>
+      </c>
+      <c r="F178">
+        <v>0.75994206495815586</v>
+      </c>
+      <c r="G178">
+        <v>0.78236903179580108</v>
+      </c>
+      <c r="H178">
+        <v>0.77387901819390625</v>
+      </c>
+      <c r="I178">
+        <v>0.77105032145725216</v>
+      </c>
+      <c r="J178">
+        <v>0.77473980729276393</v>
+      </c>
+      <c r="K178">
+        <v>0.6856128955695171</v>
+      </c>
+      <c r="L178">
+        <v>0.71646587238809811</v>
+      </c>
+      <c r="M178">
+        <v>0.67200568147231754</v>
+      </c>
+      <c r="N178">
+        <v>0.60421034583967392</v>
+      </c>
+      <c r="O178">
+        <v>0.64275667160253747</v>
+      </c>
+      <c r="P178">
+        <v>0.65186238755519688</v>
+      </c>
+      <c r="Q178">
+        <v>0.59806937607527177</v>
+      </c>
+      <c r="R178">
+        <v>0.57758381004129411</v>
+      </c>
+      <c r="S178">
+        <v>0.58587379437339626</v>
+      </c>
+      <c r="T178">
+        <v>0.59587866622622565</v>
+      </c>
+      <c r="U178">
+        <v>0.53181736484477815</v>
+      </c>
+      <c r="V178">
+        <v>0.45128471065076869</v>
+      </c>
+      <c r="W178">
+        <v>0.53746113563018971</v>
+      </c>
+      <c r="X178">
+        <v>0.54864863721203316</v>
+      </c>
+    </row>
+    <row r="179" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A179" t="s">
+        <v>35</v>
+      </c>
+      <c r="B179">
+        <v>0.2976781638234316</v>
+      </c>
+      <c r="C179">
+        <v>0.32219144582413412</v>
+      </c>
+      <c r="D179">
+        <v>0.25922042962458852</v>
+      </c>
+      <c r="E179">
+        <v>0.21452713874059057</v>
+      </c>
+      <c r="F179">
+        <v>0.22442905450337403</v>
+      </c>
+      <c r="G179">
+        <v>0.23278839649180202</v>
+      </c>
+      <c r="H179">
+        <v>0.24707302950595311</v>
+      </c>
+      <c r="I179">
+        <v>0.26522983340694134</v>
+      </c>
+      <c r="J179">
+        <v>0.26088186918268397</v>
+      </c>
+      <c r="K179">
+        <v>0.26968828398559297</v>
+      </c>
+      <c r="L179">
+        <v>0.28557877200905274</v>
+      </c>
+      <c r="M179">
+        <v>0.286702524639805</v>
+      </c>
+      <c r="N179">
+        <v>0.34086865603353944</v>
+      </c>
+      <c r="O179">
+        <v>0.30993939262520942</v>
+      </c>
+      <c r="P179">
+        <v>0.30599525417455309</v>
+      </c>
+      <c r="Q179">
+        <v>0.35540021135231642</v>
+      </c>
+      <c r="R179">
+        <v>0.36111750704091283</v>
+      </c>
+      <c r="S179">
+        <v>0.33381145447234162</v>
+      </c>
+      <c r="T179">
+        <v>0.36754237729011918</v>
+      </c>
+      <c r="U179">
+        <v>0.39149918667202238</v>
+      </c>
+      <c r="V179">
+        <v>0.39370115199065586</v>
+      </c>
+      <c r="W179">
+        <v>0.37839299918119945</v>
+      </c>
+      <c r="X179">
+        <v>0.39466156459867135</v>
+      </c>
+    </row>
+    <row r="180" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A180" t="s">
+        <v>39</v>
+      </c>
+      <c r="B180">
+        <v>0.59758823019714979</v>
+      </c>
+      <c r="C180">
+        <v>0.73380036538169091</v>
+      </c>
+      <c r="D180">
+        <v>0.75718294896377081</v>
+      </c>
+      <c r="E180">
+        <v>0.79572885713108443</v>
+      </c>
+      <c r="F180">
+        <v>0.82149472809060253</v>
+      </c>
+      <c r="G180">
+        <v>0.83809425618210642</v>
+      </c>
+      <c r="H180">
+        <v>0.83237681034049649</v>
+      </c>
+      <c r="I180">
+        <v>0.86603735375115121</v>
+      </c>
+      <c r="J180">
+        <v>0.86420564990641402</v>
+      </c>
+      <c r="K180">
+        <v>0.8169488269696058</v>
+      </c>
+      <c r="L180">
+        <v>0.83444516731060003</v>
+      </c>
+      <c r="M180">
+        <v>0.84531366443852607</v>
+      </c>
+      <c r="N180">
+        <v>0.79865957310754032</v>
+      </c>
+      <c r="O180">
+        <v>0.80666207768687392</v>
+      </c>
+      <c r="P180">
+        <v>0.84947888034778962</v>
+      </c>
+      <c r="Q180">
+        <v>0.84115104785672001</v>
+      </c>
+      <c r="R180">
+        <v>0.84298704093404275</v>
+      </c>
+      <c r="S180">
+        <v>0.8608187624840784</v>
+      </c>
+      <c r="T180">
+        <v>0.87674857001201367</v>
+      </c>
+      <c r="U180">
+        <v>0.82035964309441589</v>
+      </c>
+      <c r="V180">
+        <v>0.83582469545727878</v>
+      </c>
+      <c r="W180">
+        <v>0.83865665114468269</v>
+      </c>
+      <c r="X180">
+        <v>0.82502447230672737</v>
+      </c>
+    </row>
+    <row r="181" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A181" t="s">
+        <v>40</v>
+      </c>
+      <c r="B181">
+        <v>0.32747819821842955</v>
+      </c>
+      <c r="C181">
+        <v>0.24865417698441153</v>
+      </c>
+      <c r="D181">
+        <v>0.33396537845120833</v>
+      </c>
+      <c r="E181">
+        <v>0.35175778100306404</v>
+      </c>
+      <c r="F181">
+        <v>0.34557354182776939</v>
+      </c>
+      <c r="G181">
+        <v>0.34392607068267994</v>
+      </c>
+      <c r="H181">
+        <v>0.36528139622397499</v>
+      </c>
+      <c r="I181">
+        <v>0.3152710574796192</v>
+      </c>
+      <c r="J181">
+        <v>0.32259600398506938</v>
+      </c>
+      <c r="K181">
+        <v>0.33835662700044389</v>
+      </c>
+      <c r="L181">
+        <v>0.32324254576835298</v>
+      </c>
+      <c r="M181">
+        <v>0.3892785813467925</v>
+      </c>
+      <c r="N181">
+        <v>0.33638651172536149</v>
+      </c>
+      <c r="O181">
+        <v>0.32566602363025565</v>
+      </c>
+      <c r="P181">
+        <v>0.31424388911068774</v>
+      </c>
+      <c r="Q181">
+        <v>0.30237142059861155</v>
+      </c>
+      <c r="R181">
+        <v>0.32422909787468784</v>
+      </c>
+      <c r="S181">
+        <v>0.36084584078577098</v>
+      </c>
+      <c r="T181">
+        <v>0.35147117960042967</v>
+      </c>
+      <c r="U181">
+        <v>0.34482720875059103</v>
+      </c>
+      <c r="V181">
+        <v>0.34096968646200604</v>
+      </c>
+      <c r="W181">
+        <v>0.303312480566654</v>
+      </c>
+      <c r="X181">
+        <v>0.30827527006820737</v>
+      </c>
+    </row>
+    <row r="182" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A182" t="s">
+        <v>41</v>
+      </c>
+      <c r="B182">
+        <v>0.93055077284014898</v>
+      </c>
+      <c r="C182">
+        <v>0.92176979036846474</v>
+      </c>
+      <c r="D182">
+        <v>0.93090270830402999</v>
+      </c>
+      <c r="E182">
+        <v>0.90650735875642163</v>
+      </c>
+      <c r="F182">
+        <v>0.93193504451273468</v>
+      </c>
+      <c r="G182">
+        <v>0.92559700277139456</v>
+      </c>
+      <c r="H182">
+        <v>0.92862996382453744</v>
+      </c>
+      <c r="I182">
+        <v>0.95253076958084026</v>
+      </c>
+      <c r="J182">
+        <v>0.94923151159295749</v>
+      </c>
+      <c r="K182">
+        <v>0.93831048813289342</v>
+      </c>
+      <c r="L182">
+        <v>0.94663279866274908</v>
+      </c>
+      <c r="M182">
+        <v>0.92455929338472687</v>
+      </c>
+      <c r="N182">
+        <v>0.89761085725848577</v>
+      </c>
+      <c r="O182">
+        <v>0.94554402857871978</v>
+      </c>
+      <c r="P182">
+        <v>0.96191740343246079</v>
+      </c>
+      <c r="Q182">
+        <v>0.96057377128078236</v>
+      </c>
+      <c r="R182">
+        <v>0.96300148474471392</v>
+      </c>
+      <c r="S182">
+        <v>0.96117078606562856</v>
+      </c>
+      <c r="T182">
+        <v>0.9658988452280004</v>
+      </c>
+      <c r="U182">
+        <v>0.98116112012154111</v>
+      </c>
+      <c r="V182">
+        <v>0.9737441526495062</v>
+      </c>
+      <c r="W182">
+        <v>0.96961066266419349</v>
+      </c>
+      <c r="X182">
+        <v>0.96919609809199536</v>
+      </c>
+    </row>
+    <row r="183" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A183" t="s">
+        <v>37</v>
+      </c>
+      <c r="B183">
+        <v>0.17770960376886794</v>
+      </c>
+      <c r="C183">
+        <v>0.18702579968317939</v>
+      </c>
+      <c r="D183">
+        <v>0.22573833672768295</v>
+      </c>
+      <c r="E183">
+        <v>0.27885590814146682</v>
+      </c>
+      <c r="F183">
+        <v>0.28874673312878968</v>
+      </c>
+      <c r="G183">
+        <v>0.29107932795949315</v>
+      </c>
+      <c r="H183">
+        <v>0.17607175090710461</v>
+      </c>
+      <c r="I183">
+        <v>0.17963086160211289</v>
+      </c>
+      <c r="J183">
+        <v>0.13633459518944582</v>
+      </c>
+      <c r="K183">
+        <v>0.12367158372619123</v>
+      </c>
+      <c r="L183">
+        <v>0.12022781840666957</v>
+      </c>
+      <c r="M183">
+        <v>0.11769416203892442</v>
+      </c>
+      <c r="N183">
+        <v>0.11213559179835184</v>
+      </c>
+      <c r="O183">
+        <v>0.12804949821399444</v>
+      </c>
+      <c r="P183">
+        <v>0.14043117487364259</v>
+      </c>
+      <c r="Q183">
+        <v>0.15857743902203089</v>
+      </c>
+      <c r="R183">
+        <v>0.15603952967613555</v>
+      </c>
+      <c r="S183">
+        <v>0.14818139753302206</v>
+      </c>
+      <c r="T183">
+        <v>0.19055932297186587</v>
+      </c>
+      <c r="U183">
+        <v>0.17212289842835513</v>
+      </c>
+      <c r="V183">
+        <v>0.19882895458377348</v>
+      </c>
+      <c r="W183">
+        <v>0.18760394987071144</v>
+      </c>
+      <c r="X183">
+        <v>0.1936374291489317</v>
+      </c>
+    </row>
+    <row r="184" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A184" t="s">
+        <v>42</v>
+      </c>
+      <c r="B184">
+        <v>0.13632188121088934</v>
+      </c>
+      <c r="C184">
+        <v>0.14970242590397381</v>
+      </c>
+      <c r="D184">
+        <v>0.14744609157716865</v>
+      </c>
+      <c r="E184">
+        <v>0.14214927014395967</v>
+      </c>
+      <c r="F184">
+        <v>0.14652808905506542</v>
+      </c>
+      <c r="G184">
+        <v>0.14304529120445161</v>
+      </c>
+      <c r="H184">
+        <v>0.13370750657005651</v>
+      </c>
+      <c r="I184">
+        <v>0.13281615958504234</v>
+      </c>
+      <c r="J184">
+        <v>0.14768632750603869</v>
+      </c>
+      <c r="K184">
+        <v>0.13756610283708889</v>
+      </c>
+      <c r="L184">
+        <v>0.13305736250739209</v>
+      </c>
+      <c r="M184">
+        <v>0.12571540459727984</v>
+      </c>
+      <c r="N184">
+        <v>0.13446012107640198</v>
+      </c>
+      <c r="O184">
+        <v>0.13679152513070261</v>
+      </c>
+      <c r="P184">
+        <v>0.16238268029085035</v>
+      </c>
+      <c r="Q184">
+        <v>0.16784041844509073</v>
+      </c>
+      <c r="R184">
+        <v>0.16215903580754581</v>
+      </c>
+      <c r="S184">
+        <v>0.18512152948302751</v>
+      </c>
+      <c r="T184">
+        <v>0.18705064796094981</v>
+      </c>
+      <c r="U184">
+        <v>0.18068073124017733</v>
+      </c>
+      <c r="V184">
+        <v>0.17820298894284992</v>
+      </c>
+      <c r="W184">
+        <v>0.18108973407659021</v>
+      </c>
+      <c r="X184">
+        <v>0.18673452386067921</v>
+      </c>
+    </row>
+    <row r="185" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A185" t="s">
+        <v>43</v>
+      </c>
+      <c r="B185">
+        <v>0.27134083674790571</v>
+      </c>
+      <c r="C185">
+        <v>0.20109032913765423</v>
+      </c>
+      <c r="D185">
+        <v>0.27032988237427041</v>
+      </c>
+      <c r="E185">
+        <v>0.21516488016218727</v>
+      </c>
+      <c r="F185">
+        <v>0.25270186407012718</v>
+      </c>
+      <c r="G185">
+        <v>0.23444910653898687</v>
+      </c>
+      <c r="H185">
+        <v>0.26880235925037488</v>
+      </c>
+      <c r="I185">
+        <v>0.23918197015162743</v>
+      </c>
+      <c r="J185">
+        <v>0.2579170618823311</v>
+      </c>
+      <c r="K185">
+        <v>0.24706487882577102</v>
+      </c>
+      <c r="L185">
+        <v>0.27602866643862012</v>
+      </c>
+      <c r="M185">
+        <v>0.30125839855289749</v>
+      </c>
+      <c r="N185">
+        <v>0.27250197760281419</v>
+      </c>
+      <c r="O185">
+        <v>0.32183091392930691</v>
+      </c>
+      <c r="P185">
+        <v>0.32581370233701296</v>
+      </c>
+      <c r="Q185">
+        <v>0.30276057521699046</v>
+      </c>
+      <c r="R185">
+        <v>0.3214056499945756</v>
+      </c>
+      <c r="S185">
+        <v>0.33435117166115619</v>
+      </c>
+      <c r="T185">
+        <v>0.33262034953007769</v>
+      </c>
+      <c r="U185">
+        <v>0.32783660242943136</v>
+      </c>
+      <c r="V185">
+        <v>0.32883158242795713</v>
+      </c>
+      <c r="W185">
+        <v>0.32852552875101171</v>
+      </c>
+      <c r="X185">
+        <v>0.3539464426516985</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated BGR model - 2025-07-29 09:49
</commit_message>
<xml_diff>
--- a/VerveStacks_USA/SuppXLS/Scen_Par-NGFS.xlsx
+++ b/VerveStacks_USA/SuppXLS/Scen_Par-NGFS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_USA\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581E28BC-D44D-4C7F-911D-C9B67FAFE9CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8766AD80-8429-4865-A2F3-0DC2169488C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Veda" sheetId="1" r:id="rId1"/>
@@ -707,8 +707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:AA19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -770,8 +770,8 @@
         <v>4</v>
       </c>
       <c r="Q10" s="4">
-        <f>SUM(historical_data!F2:F16)</f>
-        <v>4011.5249889693232</v>
+        <f>historical_data!X32</f>
+        <v>4286.8900000000003</v>
       </c>
       <c r="R10" s="3" t="s">
         <v>46</v>
@@ -897,31 +897,31 @@
       </c>
       <c r="R16" s="1">
         <f>$Q$10*G16/SUM($G$16:$G$18)</f>
-        <v>13.492518112503594</v>
+        <v>14.418691427912941</v>
       </c>
       <c r="S16" s="1">
         <f>R16</f>
-        <v>13.492518112503594</v>
+        <v>14.418691427912941</v>
       </c>
       <c r="T16" s="1">
         <f t="shared" ref="T16:X16" si="0">S16</f>
-        <v>13.492518112503594</v>
+        <v>14.418691427912941</v>
       </c>
       <c r="U16" s="1">
         <f t="shared" si="0"/>
-        <v>13.492518112503594</v>
+        <v>14.418691427912941</v>
       </c>
       <c r="V16" s="1">
         <f t="shared" si="0"/>
-        <v>13.492518112503594</v>
+        <v>14.418691427912941</v>
       </c>
       <c r="W16" s="1">
         <f t="shared" si="0"/>
-        <v>13.492518112503594</v>
+        <v>14.418691427912941</v>
       </c>
       <c r="X16" s="1">
         <f t="shared" si="0"/>
-        <v>13.492518112503594</v>
+        <v>14.418691427912941</v>
       </c>
       <c r="Y16" t="s">
         <v>12</v>
@@ -964,31 +964,31 @@
       </c>
       <c r="R17" s="1">
         <f>$Q$10*G17/SUM($G$16:$G$18)</f>
-        <v>3408.724351069377</v>
+        <v>3642.7110322227509</v>
       </c>
       <c r="S17" s="1">
         <f t="shared" ref="S17:X18" si="1">R17*H17/G17</f>
-        <v>3764.7881481111208</v>
+        <v>4023.2162852368815</v>
       </c>
       <c r="T17" s="1">
         <f t="shared" si="1"/>
-        <v>3800.1229439389408</v>
+        <v>4060.9765842012021</v>
       </c>
       <c r="U17" s="1">
         <f t="shared" si="1"/>
-        <v>4075.4049837161019</v>
+        <v>4355.1549395013189</v>
       </c>
       <c r="V17" s="1">
         <f t="shared" si="1"/>
-        <v>4045.7330006292896</v>
+        <v>4323.4461684168082</v>
       </c>
       <c r="W17" s="1">
         <f t="shared" si="1"/>
-        <v>4107.5616703525393</v>
+        <v>4389.5189728188079</v>
       </c>
       <c r="X17" s="1">
         <f t="shared" si="1"/>
-        <v>4139.5450055785386</v>
+        <v>4423.697755282833</v>
       </c>
       <c r="Y17" t="s">
         <v>12</v>
@@ -1028,31 +1028,31 @@
       </c>
       <c r="R18" s="1">
         <f>$Q$10*G18/SUM($G$16:$G$18)</f>
-        <v>589.30811978744282</v>
+        <v>629.76027634933666</v>
       </c>
       <c r="S18" s="1">
         <f t="shared" si="1"/>
-        <v>599.24693398594661</v>
+        <v>640.38132528124686</v>
       </c>
       <c r="T18" s="1">
         <f t="shared" si="1"/>
-        <v>619.06677857947443</v>
+        <v>661.56167286057928</v>
       </c>
       <c r="U18" s="1">
         <f t="shared" si="1"/>
-        <v>653.24589833770085</v>
+        <v>698.08696613514246</v>
       </c>
       <c r="V18" s="1">
         <f t="shared" si="1"/>
-        <v>677.54398770090324</v>
+        <v>724.05296076228319</v>
       </c>
       <c r="W18" s="1">
         <f t="shared" si="1"/>
-        <v>698.46172456054478</v>
+        <v>746.40656374688479</v>
       </c>
       <c r="X18" s="1">
         <f t="shared" si="1"/>
-        <v>712.99435113568245</v>
+        <v>761.93676029557901</v>
       </c>
       <c r="Y18" t="s">
         <v>12</v>
@@ -1068,27 +1068,27 @@
       </c>
       <c r="S19" s="1">
         <f t="shared" ref="S19:X19" si="2">$Q$10*H16/SUM($G$16:$G$18)-S16</f>
-        <v>-1.2423517748129633</v>
+        <v>-1.3276311164887726</v>
       </c>
       <c r="T19" s="1">
         <f t="shared" si="2"/>
-        <v>72.489781465249493</v>
+        <v>77.465731890007632</v>
       </c>
       <c r="U19" s="1">
         <f t="shared" si="2"/>
-        <v>207.58831400072447</v>
+        <v>221.83789702260063</v>
       </c>
       <c r="V19" s="1">
         <f t="shared" si="2"/>
-        <v>442.65282655603329</v>
+        <v>473.0380543191738</v>
       </c>
       <c r="W19" s="1">
         <f t="shared" si="2"/>
-        <v>845.00145018499495</v>
+        <v>903.00528520807234</v>
       </c>
       <c r="X19" s="1">
         <f t="shared" si="2"/>
-        <v>1292.1614134124429</v>
+        <v>1380.8598617172984</v>
       </c>
       <c r="Y19" t="s">
         <v>12</v>
@@ -3466,19 +3466,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:Z87"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="7.796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.73046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="19.1328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.53125" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.73046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.73046875" bestFit="1" customWidth="1"/>
+    <col min="14" max="19" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.73046875" bestFit="1" customWidth="1"/>
+    <col min="21" max="23" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.73046875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="7.73046875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="5.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="15.75" x14ac:dyDescent="0.5">

</xml_diff>

<commit_message>
Updated USA model - 2025-08-03 14:44
</commit_message>
<xml_diff>
--- a/VerveStacks_USA/SuppXLS/Scen_Par-NGFS.xlsx
+++ b/VerveStacks_USA/SuppXLS/Scen_Par-NGFS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_USA\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9C87685-FD89-4023-A7F1-AC8D55C2CA25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54907F3E-7D86-443B-B5D7-99858B6BF574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Veda" sheetId="1" r:id="rId1"/>
@@ -36,6 +36,9 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="65">
+  <si>
+    <t>~Inputcell: 3</t>
+  </si>
   <si>
     <t>Delayed transition</t>
   </si>
@@ -227,9 +230,6 @@
   </si>
   <si>
     <t>Import</t>
-  </si>
-  <si>
-    <t>~Inputcell: 2-3</t>
   </si>
 </sst>
 </file>
@@ -725,8 +725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:AA25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Y26" sqref="Y26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -742,18 +742,18 @@
   <sheetData>
     <row r="2" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
-        <v>64</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="2:27" x14ac:dyDescent="0.45">
       <c r="C5" s="2" t="str">
         <f>VLOOKUP(B3,$B$7:$C$14,2,FALSE)</f>
-        <v>Net Zero 2050</v>
+        <v>Nationally Determined Contributions (NDCs)</v>
       </c>
     </row>
     <row r="7" spans="2:27" x14ac:dyDescent="0.45">
@@ -761,7 +761,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:27" x14ac:dyDescent="0.45">
@@ -769,7 +769,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="2:27" x14ac:dyDescent="0.45">
@@ -777,7 +777,7 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="2:27" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -785,14 +785,14 @@
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Q10" s="4">
         <f>historical_data!X32</f>
         <v>4286.8900000000003</v>
       </c>
       <c r="R10" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="2:27" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
@@ -800,7 +800,7 @@
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="2:27" x14ac:dyDescent="0.45">
@@ -808,7 +808,7 @@
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="2:27" x14ac:dyDescent="0.45">
@@ -816,12 +816,12 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="2:27" ht="17.649999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="Q14" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="2:27" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -854,7 +854,7 @@
         <v>2050</v>
       </c>
       <c r="Q15" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R15" s="5">
         <v>2022</v>
@@ -878,207 +878,207 @@
         <v>2050</v>
       </c>
       <c r="Y15" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="2:27" x14ac:dyDescent="0.45">
       <c r="G16">
         <f>SUMIFS(iamc_data!F$2:F$50,iamc_data!$O$2:$O$50,Veda!$Q16,iamc_data!$B$2:$B$50,Veda!$C$5)</f>
-        <v>4.7699999999999999E-2</v>
+        <v>4.6699999999999998E-2</v>
       </c>
       <c r="H16">
         <f>SUMIFS(iamc_data!G$2:G$50,iamc_data!$O$2:$O$50,Veda!$Q16,iamc_data!$B$2:$B$50,Veda!$C$5)</f>
-        <v>4.4200000000000003E-2</v>
+        <v>4.24E-2</v>
       </c>
       <c r="I16">
         <f>SUMIFS(iamc_data!H$2:H$50,iamc_data!$O$2:$O$50,Veda!$Q16,iamc_data!$B$2:$B$50,Veda!$C$5)</f>
-        <v>0.32069999999999999</v>
+        <v>0.29759999999999998</v>
       </c>
       <c r="J16">
         <f>SUMIFS(iamc_data!I$2:I$50,iamc_data!$O$2:$O$50,Veda!$Q16,iamc_data!$B$2:$B$50,Veda!$C$5)</f>
-        <v>0.80020000000000002</v>
+        <v>0.76519999999999999</v>
       </c>
       <c r="K16">
         <f>SUMIFS(iamc_data!J$2:J$50,iamc_data!$O$2:$O$50,Veda!$Q16,iamc_data!$B$2:$B$50,Veda!$C$5)</f>
-        <v>1.6148</v>
+        <v>1.5788</v>
       </c>
       <c r="L16">
         <f>SUMIFS(iamc_data!K$2:K$50,iamc_data!$O$2:$O$50,Veda!$Q16,iamc_data!$B$2:$B$50,Veda!$C$5)</f>
-        <v>3.0192999999999999</v>
+        <v>2.9714</v>
       </c>
       <c r="M16">
         <f>SUMIFS(iamc_data!L$2:L$50,iamc_data!$O$2:$O$50,Veda!$Q16,iamc_data!$B$2:$B$50,Veda!$C$5)</f>
-        <v>5.0453000000000001</v>
+        <v>4.5190999999999999</v>
       </c>
       <c r="Q16" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R16" s="1">
         <f>$Q$10*G16/SUM($G$16:$G$18)</f>
-        <v>14.643177557377637</v>
+        <v>14.418691427912941</v>
       </c>
       <c r="S16" s="1">
         <f>R16</f>
-        <v>14.643177557377637</v>
+        <v>14.418691427912941</v>
       </c>
       <c r="T16" s="1">
         <f t="shared" ref="T16:X16" si="0">S16</f>
-        <v>14.643177557377637</v>
+        <v>14.418691427912941</v>
       </c>
       <c r="U16" s="1">
         <f t="shared" si="0"/>
-        <v>14.643177557377637</v>
+        <v>14.418691427912941</v>
       </c>
       <c r="V16" s="1">
         <f t="shared" si="0"/>
-        <v>14.643177557377637</v>
+        <v>14.418691427912941</v>
       </c>
       <c r="W16" s="1">
         <f t="shared" si="0"/>
-        <v>14.643177557377637</v>
+        <v>14.418691427912941</v>
       </c>
       <c r="X16" s="1">
         <f t="shared" si="0"/>
-        <v>14.643177557377637</v>
+        <v>14.418691427912941</v>
       </c>
       <c r="Y16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="AA16" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="7:26" x14ac:dyDescent="0.45">
       <c r="G17">
         <f>SUMIFS(iamc_data!F$2:F$50,iamc_data!$O$2:$O$50,Veda!$Q17,iamc_data!$B$2:$B$50,Veda!$C$5)</f>
-        <v>11.848699999999999</v>
+        <v>11.7982</v>
       </c>
       <c r="H17">
         <f>SUMIFS(iamc_data!G$2:G$50,iamc_data!$O$2:$O$50,Veda!$Q17,iamc_data!$B$2:$B$50,Veda!$C$5)</f>
-        <v>13.113099999999999</v>
+        <v>13.0306</v>
       </c>
       <c r="I17">
         <f>SUMIFS(iamc_data!H$2:H$50,iamc_data!$O$2:$O$50,Veda!$Q17,iamc_data!$B$2:$B$50,Veda!$C$5)</f>
-        <v>14.072900000000001</v>
+        <v>13.152900000000001</v>
       </c>
       <c r="J17">
         <f>SUMIFS(iamc_data!I$2:I$50,iamc_data!$O$2:$O$50,Veda!$Q17,iamc_data!$B$2:$B$50,Veda!$C$5)</f>
-        <v>15.4162</v>
+        <v>14.105700000000001</v>
       </c>
       <c r="K17">
         <f>SUMIFS(iamc_data!J$2:J$50,iamc_data!$O$2:$O$50,Veda!$Q17,iamc_data!$B$2:$B$50,Veda!$C$5)</f>
-        <v>16.447299999999998</v>
+        <v>14.003</v>
       </c>
       <c r="L17">
         <f>SUMIFS(iamc_data!K$2:K$50,iamc_data!$O$2:$O$50,Veda!$Q17,iamc_data!$B$2:$B$50,Veda!$C$5)</f>
-        <v>17.144300000000001</v>
+        <v>14.217000000000001</v>
       </c>
       <c r="M17">
         <f>SUMIFS(iamc_data!L$2:L$50,iamc_data!$O$2:$O$50,Veda!$Q17,iamc_data!$B$2:$B$50,Veda!$C$5)</f>
-        <v>17.7699</v>
+        <v>14.3277</v>
       </c>
       <c r="Q17" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="R17" s="1">
         <f>$Q$10*G17/SUM($G$16:$G$18)</f>
-        <v>3637.3714449496938</v>
+        <v>3642.7110322227509</v>
       </c>
       <c r="S17" s="1">
         <f t="shared" ref="S17:X18" si="1">R17*H17/G17</f>
-        <v>4025.5230949192596</v>
+        <v>4023.2162852368815</v>
       </c>
       <c r="T17" s="1">
         <f t="shared" si="1"/>
-        <v>4320.1671582226363</v>
+        <v>4060.9765842012021</v>
       </c>
       <c r="U17" s="1">
         <f t="shared" si="1"/>
-        <v>4732.5399132084931</v>
+        <v>4355.1549395013189</v>
       </c>
       <c r="V17" s="1">
         <f t="shared" si="1"/>
-        <v>5049.0719966343222</v>
+        <v>4323.4461684168082</v>
       </c>
       <c r="W17" s="1">
         <f t="shared" si="1"/>
-        <v>5263.0404401876194</v>
+        <v>4389.5189728188079</v>
       </c>
       <c r="X17" s="1">
         <f t="shared" si="1"/>
-        <v>5455.0901651330159</v>
+        <v>4423.697755282833</v>
       </c>
       <c r="Y17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="7:26" x14ac:dyDescent="0.45">
       <c r="G18">
         <f>SUMIFS(iamc_data!F$2:F$50,iamc_data!$O$2:$O$50,Veda!$Q18,iamc_data!$B$2:$B$50,Veda!$C$5)</f>
-        <v>2.0680999999999998</v>
+        <v>2.0396999999999998</v>
       </c>
       <c r="H18">
         <f>SUMIFS(iamc_data!G$2:G$50,iamc_data!$O$2:$O$50,Veda!$Q18,iamc_data!$B$2:$B$50,Veda!$C$5)</f>
-        <v>2.1147</v>
+        <v>2.0741000000000001</v>
       </c>
       <c r="I18">
         <f>SUMIFS(iamc_data!H$2:H$50,iamc_data!$O$2:$O$50,Veda!$Q18,iamc_data!$B$2:$B$50,Veda!$C$5)</f>
-        <v>2.4839000000000002</v>
+        <v>2.1427</v>
       </c>
       <c r="J18">
         <f>SUMIFS(iamc_data!I$2:I$50,iamc_data!$O$2:$O$50,Veda!$Q18,iamc_data!$B$2:$B$50,Veda!$C$5)</f>
-        <v>2.8763000000000001</v>
+        <v>2.2610000000000001</v>
       </c>
       <c r="K18">
         <f>SUMIFS(iamc_data!J$2:J$50,iamc_data!$O$2:$O$50,Veda!$Q18,iamc_data!$B$2:$B$50,Veda!$C$5)</f>
-        <v>3.2075</v>
+        <v>2.3451</v>
       </c>
       <c r="L18">
         <f>SUMIFS(iamc_data!K$2:K$50,iamc_data!$O$2:$O$50,Veda!$Q18,iamc_data!$B$2:$B$50,Veda!$C$5)</f>
-        <v>3.5516000000000001</v>
+        <v>2.4175</v>
       </c>
       <c r="M18">
         <f>SUMIFS(iamc_data!L$2:L$50,iamc_data!$O$2:$O$50,Veda!$Q18,iamc_data!$B$2:$B$50,Veda!$C$5)</f>
-        <v>3.9205000000000001</v>
+        <v>2.4678</v>
       </c>
       <c r="Q18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="R18" s="1">
         <f>$Q$10*G18/SUM($G$16:$G$18)</f>
-        <v>634.87537749292858</v>
+        <v>629.76027634933666</v>
       </c>
       <c r="S18" s="1">
         <f t="shared" si="1"/>
-        <v>649.18087171040872</v>
+        <v>640.38132528124686</v>
       </c>
       <c r="T18" s="1">
         <f t="shared" si="1"/>
-        <v>762.51967997422059</v>
+        <v>661.56167286057928</v>
       </c>
       <c r="U18" s="1">
         <f t="shared" si="1"/>
-        <v>882.9805368613271</v>
+        <v>698.08696613514246</v>
       </c>
       <c r="V18" s="1">
         <f t="shared" si="1"/>
-        <v>984.65392065594915</v>
+        <v>724.05296076228319</v>
       </c>
       <c r="W18" s="1">
         <f t="shared" si="1"/>
-        <v>1090.2874090730068</v>
+        <v>746.40656374688479</v>
       </c>
       <c r="X18" s="1">
         <f t="shared" si="1"/>
-        <v>1203.5341218804829</v>
+        <v>761.93676029557901</v>
       </c>
       <c r="Y18" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="7:26" x14ac:dyDescent="0.45">
       <c r="Q19" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="R19" s="1">
         <f>$Q$10*G16/SUM($G$16:$G$18)-R16</f>
@@ -1086,40 +1086,40 @@
       </c>
       <c r="S19" s="1">
         <f t="shared" ref="S19:X19" si="2">$Q$10*H16/SUM($G$16:$G$18)-S16</f>
-        <v>-1.0744469905832634</v>
+        <v>-1.3276311164887726</v>
       </c>
       <c r="T19" s="1">
         <f t="shared" si="2"/>
-        <v>83.80686526549465</v>
+        <v>77.465731890007632</v>
       </c>
       <c r="U19" s="1">
         <f t="shared" si="2"/>
-        <v>231.00610297540194</v>
+        <v>221.83789702260063</v>
       </c>
       <c r="V19" s="1">
         <f t="shared" si="2"/>
-        <v>481.07596541229555</v>
+        <v>473.0380543191738</v>
       </c>
       <c r="W19" s="1">
         <f t="shared" si="2"/>
-        <v>912.23619349063711</v>
+        <v>903.00528520807234</v>
       </c>
       <c r="X19" s="1">
         <f t="shared" si="2"/>
-        <v>1534.1875086111215</v>
+        <v>1380.8598617172984</v>
       </c>
       <c r="Y19" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="7:26" ht="17.649999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="Q22" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="7:26" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="Q23" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="R23" s="5">
         <f>R15</f>
@@ -1150,15 +1150,15 @@
         <v>2050</v>
       </c>
       <c r="Y23" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="Z23" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="7:26" x14ac:dyDescent="0.45">
       <c r="Q24" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="R24" s="1">
         <f>historical_data!Y87</f>
@@ -1169,15 +1169,15 @@
         <v>16.25</v>
       </c>
       <c r="Y24" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="Z24" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="7:26" x14ac:dyDescent="0.45">
       <c r="Q25" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="R25" s="1">
         <f>historical_data!Y88</f>
@@ -1188,10 +1188,10 @@
         <v>54.65</v>
       </c>
       <c r="Y25" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="Z25" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1211,19 +1211,19 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F1">
         <v>2020</v>
@@ -1247,30 +1247,30 @@
         <v>2050</v>
       </c>
       <c r="M1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F2">
         <v>2.0274999999999999</v>
@@ -1294,30 +1294,30 @@
         <v>2.9030999999999998</v>
       </c>
       <c r="M2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F3">
         <v>2.0680999999999998</v>
@@ -1341,30 +1341,30 @@
         <v>3.9205000000000001</v>
       </c>
       <c r="M3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F4">
         <v>4.6699999999999998E-2</v>
@@ -1388,30 +1388,30 @@
         <v>4.5190999999999999</v>
       </c>
       <c r="M4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N4" t="s">
         <v>28</v>
       </c>
-      <c r="N4" t="s">
-        <v>27</v>
-      </c>
       <c r="O4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F5">
         <v>11.7982</v>
@@ -1435,30 +1435,30 @@
         <v>14.3277</v>
       </c>
       <c r="M5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F6">
         <v>2.0396999999999998</v>
@@ -1482,30 +1482,30 @@
         <v>2.4678</v>
       </c>
       <c r="M6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F7">
         <v>2.0451000000000001</v>
@@ -1529,30 +1529,30 @@
         <v>2.5503</v>
       </c>
       <c r="M7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F8">
         <v>11.8245</v>
@@ -1576,30 +1576,30 @@
         <v>15.2393</v>
       </c>
       <c r="M8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F9">
         <v>4.6699999999999998E-2</v>
@@ -1623,30 +1623,30 @@
         <v>4.7785000000000002</v>
       </c>
       <c r="M9" t="s">
+        <v>29</v>
+      </c>
+      <c r="N9" t="s">
         <v>28</v>
       </c>
-      <c r="N9" t="s">
-        <v>27</v>
-      </c>
       <c r="O9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F10">
         <v>4.6600000000000003E-2</v>
@@ -1670,30 +1670,30 @@
         <v>0.87119999999999997</v>
       </c>
       <c r="M10" t="s">
+        <v>29</v>
+      </c>
+      <c r="N10" t="s">
         <v>28</v>
       </c>
-      <c r="N10" t="s">
-        <v>27</v>
-      </c>
       <c r="O10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F11">
         <v>11.848699999999999</v>
@@ -1717,30 +1717,30 @@
         <v>17.7699</v>
       </c>
       <c r="M11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F12">
         <v>2.0367000000000002</v>
@@ -1764,30 +1764,30 @@
         <v>2.4895999999999998</v>
       </c>
       <c r="M12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F13">
         <v>11.7905</v>
@@ -1811,30 +1811,30 @@
         <v>14.9033</v>
       </c>
       <c r="M13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F14">
         <v>4.7699999999999999E-2</v>
@@ -1858,30 +1858,30 @@
         <v>5.0453000000000001</v>
       </c>
       <c r="M14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N14" t="s">
         <v>28</v>
       </c>
-      <c r="N14" t="s">
-        <v>27</v>
-      </c>
       <c r="O14" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D15" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F15">
         <v>11.7866</v>
@@ -1905,30 +1905,30 @@
         <v>15.8461</v>
       </c>
       <c r="M15" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F16">
         <v>2.0655999999999999</v>
@@ -1952,30 +1952,30 @@
         <v>1.6294999999999999</v>
       </c>
       <c r="M16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D17" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E17" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F17">
         <v>4.6199999999999998E-2</v>
@@ -1999,30 +1999,30 @@
         <v>3.1082999999999998</v>
       </c>
       <c r="M17" t="s">
+        <v>29</v>
+      </c>
+      <c r="N17" t="s">
         <v>28</v>
       </c>
-      <c r="N17" t="s">
-        <v>27</v>
-      </c>
       <c r="O17" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D18" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E18" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F18">
         <v>11.803900000000001</v>
@@ -2046,30 +2046,30 @@
         <v>14.361800000000001</v>
       </c>
       <c r="M18" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N18" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O18" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C19" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D19" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E19" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F19">
         <v>2.0305</v>
@@ -2093,30 +2093,30 @@
         <v>2.7471000000000001</v>
       </c>
       <c r="M19" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N19" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D20" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E20" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F20">
         <v>11.845000000000001</v>
@@ -2140,30 +2140,30 @@
         <v>9.4115000000000002</v>
       </c>
       <c r="M20" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O20" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D21" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E21" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F21">
         <v>4.9599999999999998E-2</v>
@@ -2187,30 +2187,30 @@
         <v>4.8047000000000004</v>
       </c>
       <c r="M21" t="s">
+        <v>29</v>
+      </c>
+      <c r="N21" t="s">
         <v>28</v>
       </c>
-      <c r="N21" t="s">
-        <v>27</v>
-      </c>
       <c r="O21" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E22" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F22">
         <v>4.6100000000000002E-2</v>
@@ -2234,30 +2234,30 @@
         <v>3.097</v>
       </c>
       <c r="M22" t="s">
+        <v>29</v>
+      </c>
+      <c r="N22" t="s">
         <v>28</v>
       </c>
-      <c r="N22" t="s">
-        <v>27</v>
-      </c>
       <c r="O22" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D23" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E23" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F23">
         <v>4.4684999999999997</v>
@@ -2281,30 +2281,30 @@
         <v>39.630600000000001</v>
       </c>
       <c r="M23" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N23" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O23" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D24" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E24" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F24">
         <v>2.4399000000000002</v>
@@ -2328,30 +2328,30 @@
         <v>9.2357999999999993</v>
       </c>
       <c r="M24" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N24" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O24" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D25" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E25" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F25">
         <v>3.6044999999999998</v>
@@ -2375,30 +2375,30 @@
         <v>8.3611000000000004</v>
       </c>
       <c r="M25" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="N25" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O25" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D26" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E26" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F26">
         <v>3.6044999999999998</v>
@@ -2422,30 +2422,30 @@
         <v>5.6074000000000002</v>
       </c>
       <c r="M26" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="N26" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O26" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C27" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D27" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E27" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F27">
         <v>2.4399000000000002</v>
@@ -2469,30 +2469,30 @@
         <v>5.8563999999999998</v>
       </c>
       <c r="M27" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N27" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O27" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C28" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D28" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E28" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F28">
         <v>3.5491999999999999</v>
@@ -2516,30 +2516,30 @@
         <v>5.7312000000000003</v>
       </c>
       <c r="M28" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N28" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O28" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B29" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D29" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E29" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F29">
         <v>4.4684999999999997</v>
@@ -2563,30 +2563,30 @@
         <v>9.1260999999999992</v>
       </c>
       <c r="M29" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N29" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O29" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B30" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C30" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D30" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E30" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F30">
         <v>2.4399000000000002</v>
@@ -2610,30 +2610,30 @@
         <v>2.8115999999999999</v>
       </c>
       <c r="M30" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N30" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O30" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B31" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D31" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E31" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F31">
         <v>3.5491999999999999</v>
@@ -2657,30 +2657,30 @@
         <v>4.6989999999999998</v>
       </c>
       <c r="M31" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N31" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O31" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B32" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C32" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D32" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E32" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F32">
         <v>4.4684999999999997</v>
@@ -2704,30 +2704,30 @@
         <v>20.0123</v>
       </c>
       <c r="M32" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N32" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O32" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B33" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C33" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D33" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E33" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F33">
         <v>4.4684999999999997</v>
@@ -2751,30 +2751,30 @@
         <v>7.2515999999999998</v>
       </c>
       <c r="M33" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N33" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O33" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B34" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C34" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D34" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E34" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F34">
         <v>3.6044999999999998</v>
@@ -2798,30 +2798,30 @@
         <v>5.3502999999999998</v>
       </c>
       <c r="M34" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="N34" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O34" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B35" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D35" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E35" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F35">
         <v>4.4684999999999997</v>
@@ -2845,30 +2845,30 @@
         <v>12.1509</v>
       </c>
       <c r="M35" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N35" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O35" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B36" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D36" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E36" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F36">
         <v>2.4399000000000002</v>
@@ -2892,30 +2892,30 @@
         <v>3.4154</v>
       </c>
       <c r="M36" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N36" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O36" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B37" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D37" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E37" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F37">
         <v>3.6044999999999998</v>
@@ -2939,30 +2939,30 @@
         <v>5.8547000000000002</v>
       </c>
       <c r="M37" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="N37" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O37" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B38" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D38" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E38" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F38">
         <v>3.5491999999999999</v>
@@ -2986,30 +2986,30 @@
         <v>6.8101000000000003</v>
       </c>
       <c r="M38" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N38" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O38" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B39" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C39" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D39" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E39" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F39">
         <v>4.4684999999999997</v>
@@ -3033,30 +3033,30 @@
         <v>12.518000000000001</v>
       </c>
       <c r="M39" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N39" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O39" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B40" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C40" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D40" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E40" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F40">
         <v>2.4399000000000002</v>
@@ -3080,30 +3080,30 @@
         <v>1.1781999999999999</v>
       </c>
       <c r="M40" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N40" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O40" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B41" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C41" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D41" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E41" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F41">
         <v>3.5491999999999999</v>
@@ -3127,30 +3127,30 @@
         <v>6.2126000000000001</v>
       </c>
       <c r="M41" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N41" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O41" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B42" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C42" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D42" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E42" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F42">
         <v>3.6044999999999998</v>
@@ -3174,30 +3174,30 @@
         <v>5.7249999999999996</v>
       </c>
       <c r="M42" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="N42" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O42" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B43" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C43" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D43" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E43" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F43">
         <v>4.4684999999999997</v>
@@ -3221,30 +3221,30 @@
         <v>4.3316999999999997</v>
       </c>
       <c r="M43" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N43" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O43" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B44" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C44" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D44" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E44" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F44">
         <v>2.4399000000000002</v>
@@ -3268,30 +3268,30 @@
         <v>2.6955</v>
       </c>
       <c r="M44" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N44" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O44" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B45" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C45" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D45" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E45" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F45">
         <v>3.6044999999999998</v>
@@ -3315,30 +3315,30 @@
         <v>5.0925000000000002</v>
       </c>
       <c r="M45" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="N45" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O45" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B46" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C46" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D46" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E46" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F46">
         <v>3.5491999999999999</v>
@@ -3362,30 +3362,30 @@
         <v>6.5091999999999999</v>
       </c>
       <c r="M46" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N46" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O46" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B47" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C47" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D47" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E47" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F47">
         <v>3.6044999999999998</v>
@@ -3409,30 +3409,30 @@
         <v>6.1596000000000002</v>
       </c>
       <c r="M47" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="N47" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O47" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B48" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C48" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D48" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E48" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F48">
         <v>2.4399000000000002</v>
@@ -3456,30 +3456,30 @@
         <v>1.796</v>
       </c>
       <c r="M48" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N48" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O48" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B49" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C49" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D49" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E49" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F49">
         <v>3.5491999999999999</v>
@@ -3503,30 +3503,30 @@
         <v>6.8875999999999999</v>
       </c>
       <c r="M49" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N49" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O49" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B50" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C50" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D50" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E50" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F50">
         <v>3.5491999999999999</v>
@@ -3550,13 +3550,13 @@
         <v>3.3336999999999999</v>
       </c>
       <c r="M50" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N50" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O50" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -3568,7 +3568,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:Z88"/>
     </sheetView>
   </sheetViews>
@@ -3589,12 +3589,12 @@
   <sheetData>
     <row r="1" spans="1:25" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A1" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A2" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B2" s="8">
         <v>2000</v>
@@ -3671,7 +3671,7 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B3" s="9">
         <v>0.89062522319196646</v>
@@ -3748,7 +3748,7 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B4" s="9">
         <v>0.67155351143519759</v>
@@ -3825,7 +3825,7 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B5" s="9">
         <v>0.43459414324342821</v>
@@ -3902,7 +3902,7 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B6" s="9">
         <v>0.38842417421564296</v>
@@ -3979,7 +3979,7 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B7" s="9">
         <v>0.87942471166058678</v>
@@ -4056,7 +4056,7 @@
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B8" s="9">
         <v>0.15384240024907564</v>
@@ -4133,7 +4133,7 @@
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B9" s="9">
         <v>9.4806903490441935E-2</v>
@@ -4210,7 +4210,7 @@
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B10" s="9">
         <v>0.26812094700894057</v>
@@ -4287,12 +4287,12 @@
     </row>
     <row r="15" spans="1:25" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A15" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A16" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B16" s="8">
         <v>2000</v>
@@ -4366,7 +4366,7 @@
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B17" s="9">
         <v>0.94365811868302962</v>
@@ -4440,7 +4440,7 @@
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B18" s="9">
         <v>0.75717051282625658</v>
@@ -4514,7 +4514,7 @@
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B19" s="9">
         <v>0.2976781638234316</v>
@@ -4588,7 +4588,7 @@
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B20" s="9">
         <v>0.59758823019714979</v>
@@ -4662,7 +4662,7 @@
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B21" s="9">
         <v>0.32747819821842955</v>
@@ -4736,7 +4736,7 @@
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B22" s="9">
         <v>0.93055077284014898</v>
@@ -4810,7 +4810,7 @@
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B23" s="9">
         <v>0.17770960376886794</v>
@@ -4884,7 +4884,7 @@
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B24" s="9">
         <v>0.13632188121088934</v>
@@ -4958,7 +4958,7 @@
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B25" s="9">
         <v>0.27134083674790571</v>
@@ -5032,12 +5032,12 @@
     </row>
     <row r="30" spans="1:25" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A30" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A31" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B31" s="8">
         <v>2000</v>
@@ -5114,7 +5114,7 @@
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A32" s="10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B32" s="10">
         <v>3802.0999999999995</v>
@@ -5191,7 +5191,7 @@
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B33" s="11">
         <v>74.819999999999993</v>
@@ -5268,7 +5268,7 @@
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B34" s="11">
         <v>1966.27</v>
@@ -5345,7 +5345,7 @@
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B35" s="11">
         <v>614.99</v>
@@ -5422,7 +5422,7 @@
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B36" s="11">
         <v>270.02999999999997</v>
@@ -5499,7 +5499,7 @@
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B37" s="11">
         <v>753.89</v>
@@ -5576,7 +5576,7 @@
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B38" s="11">
         <v>116.02</v>
@@ -5653,7 +5653,7 @@
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B39" s="11">
         <v>0.49</v>
@@ -5730,7 +5730,7 @@
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B40" s="11">
         <v>5.59</v>
@@ -5807,12 +5807,12 @@
     </row>
     <row r="44" spans="1:25" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A44" s="7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="45" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A45" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B45" s="8">
         <v>2000</v>
@@ -5886,7 +5886,7 @@
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A46" s="10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B46" s="10">
         <v>4052.6670010000003</v>
@@ -5960,7 +5960,7 @@
     </row>
     <row r="47" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B47" s="11">
         <v>56.180000999999997</v>
@@ -6034,7 +6034,7 @@
     </row>
     <row r="48" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B48" s="11">
         <v>2129.498</v>
@@ -6108,7 +6108,7 @@
     </row>
     <row r="49" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B49" s="11">
         <v>634.29</v>
@@ -6182,7 +6182,7 @@
     </row>
     <row r="50" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B50" s="11">
         <v>14.621</v>
@@ -6256,7 +6256,7 @@
     </row>
     <row r="51" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B51" s="11">
         <v>279.98599999999999</v>
@@ -6330,7 +6330,7 @@
     </row>
     <row r="52" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B52" s="11">
         <v>797.71799999999996</v>
@@ -6404,7 +6404,7 @@
     </row>
     <row r="53" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B53" s="11">
         <v>134.01499999999999</v>
@@ -6478,7 +6478,7 @@
     </row>
     <row r="54" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B54" s="11">
         <v>0.70900000000000007</v>
@@ -6552,7 +6552,7 @@
     </row>
     <row r="55" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B55" s="11">
         <v>5.65</v>
@@ -6626,12 +6626,12 @@
     </row>
     <row r="59" spans="1:25" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A59" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="60" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A60" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B60" s="8">
         <v>2000</v>
@@ -6708,7 +6708,7 @@
     </row>
     <row r="61" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B61" s="11">
         <v>9.59</v>
@@ -6785,7 +6785,7 @@
     </row>
     <row r="62" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B62" s="11">
         <v>334.24</v>
@@ -6862,7 +6862,7 @@
     </row>
     <row r="63" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B63" s="11">
         <v>161.54</v>
@@ -6939,7 +6939,7 @@
     </row>
     <row r="64" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B64" s="11">
         <v>79.36</v>
@@ -7016,7 +7016,7 @@
     </row>
     <row r="65" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B65" s="11">
         <v>97.86</v>
@@ -7093,7 +7093,7 @@
     </row>
     <row r="66" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B66" s="11">
         <v>86.09</v>
@@ -7170,7 +7170,7 @@
     </row>
     <row r="67" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B67" s="11">
         <v>0.59</v>
@@ -7247,7 +7247,7 @@
     </row>
     <row r="68" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B68" s="11">
         <v>2.38</v>
@@ -7324,12 +7324,12 @@
     </row>
     <row r="71" spans="1:26" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A71" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="72" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A72" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B72" s="8">
         <v>2000</v>
@@ -7409,7 +7409,7 @@
     </row>
     <row r="73" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B73" s="11">
         <v>6.796149999999999</v>
@@ -7489,7 +7489,7 @@
     </row>
     <row r="74" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B74" s="11">
         <v>321.05500000000001</v>
@@ -7569,7 +7569,7 @@
     </row>
     <row r="75" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B75" s="11">
         <v>243.24100000000001</v>
@@ -7649,7 +7649,7 @@
     </row>
     <row r="76" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B76" s="11">
         <v>2.7930000000000001</v>
@@ -7729,7 +7729,7 @@
     </row>
     <row r="77" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B77" s="11">
         <v>97.600000000000009</v>
@@ -7809,7 +7809,7 @@
     </row>
     <row r="78" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B78" s="11">
         <v>97.86</v>
@@ -7889,7 +7889,7 @@
     </row>
     <row r="79" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B79" s="11">
         <v>86.087164999999999</v>
@@ -7969,7 +7969,7 @@
     </row>
     <row r="80" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B80" s="11">
         <v>0.59371299999999994</v>
@@ -8049,7 +8049,7 @@
     </row>
     <row r="81" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B81" s="11">
         <v>2.3769999999999998</v>
@@ -8129,15 +8129,15 @@
     </row>
     <row r="85" spans="1:26" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A85" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="86" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A86" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C86" s="8">
         <v>2000</v>
@@ -8214,10 +8214,10 @@
     </row>
     <row r="87" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B87" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C87" s="11">
         <v>14.7</v>
@@ -8294,10 +8294,10 @@
     </row>
     <row r="88" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B88" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C88" s="11">
         <v>48.6</v>

</xml_diff>